<commit_message>
Adding the generated outputs to track changes between mods.
</commit_message>
<xml_diff>
--- a/examples/for_equinor/for_equinor-monopile/15mw/20m/outputs/monotow_output.xlsx
+++ b/examples/for_equinor/for_equinor-monopile/15mw/20m/outputs/monotow_output.xlsx
@@ -914,8 +914,8 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[[0.05045858 0.05942742 0.14509201 0.05637616 0.13109693 0.04393484
-  0.12102924]]</t>
+          <t>[[0.05031772 0.0595708  0.14492055 0.05628306 0.13110318 0.04395645
+  0.12123106]]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>[2.65900098]</t>
+          <t>[2.66846269]</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>[[0.08000787 0.05507333 0.01943857 0.008654   0.01654327]]</t>
+          <t>[[0.08002922 0.055112   0.01937491 0.00871629 0.01648097]]</t>
         </is>
       </c>
       <c r="E138" t="inlineStr"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          9.99992573  6.00000003]</t>
+          <t>[10.         10.         10.         10.          6.00000255]</t>
         </is>
       </c>
       <c r="E139" t="inlineStr"/>
@@ -4573,10 +4573,10 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          63274.56438251
-  63567.52329466  64449.93152488  65932.48512269  68033.35918549
-  70778.7656079   74203.80685615  83285.51715675  95797.25155505
- 112544.89762894      0.              0.              0.
+          <t>[     0.              0.              0.          63274.56439359
+  63567.52330231  64449.93152909  65932.48512338  68033.35918758
+  70778.76561151  74203.80686143  83285.51716102  95797.25155807
+ 112544.89763027      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -4969,10 +4969,10 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          63274.56438251
-  63567.52329466  64449.93152488  65932.48512269  68033.35918549
-  70778.7656079   74203.80685615  83285.51715675  95797.25155505
- 112544.89762894      0.              0.              0.
+          <t>[     0.              0.              0.          63274.56439359
+  63567.52330231  64449.93152909  65932.48512338  68033.35918758
+  70778.76561151  74203.80686143  83285.51716102  95797.25155807
+ 112544.89763027      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -5115,10 +5115,10 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -63274.56438251
-  -63567.52329466  -64449.93152488  -65932.48512269  -68033.35918549
-  -70778.7656079   -74203.80685615  -83285.51715675  -95797.25155505
- -112544.89762894       0.               0.               0.
+          <t>[      0.               0.               0.          -63274.56439359
+  -63567.52330231  -64449.93152909  -65932.48512338  -68033.35918758
+  -70778.76561151  -74203.80686143  -83285.51716102  -95797.25155807
+ -112544.89763027       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -5192,7 +5192,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>[0.054943   0.10225972 0.10073409 0.09373654 0.08751588 0.08248204]</t>
+          <t>[0.05494426 0.10224567 0.1006018  0.09369312 0.08752982 0.08259375]</t>
         </is>
       </c>
       <c r="E205" t="inlineStr"/>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>[0.054943   0.10225972 0.10073409 0.09373654 0.08751588 0.08248204]</t>
+          <t>[0.05494426 0.10224567 0.1006018  0.09369312 0.08752982 0.08259375]</t>
         </is>
       </c>
       <c r="E209" t="inlineStr"/>
@@ -5544,9 +5544,9 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>[0.054943   0.054943   0.054943   0.10225972 0.10225972 0.10225972
- 0.10073409 0.10073409 0.10073409 0.09373654 0.09373654 0.09373654
- 0.08751588 0.08751588 0.08751588 0.08248204 0.08248204 0.08248204]</t>
+          <t>[0.05494426 0.05494426 0.05494426 0.10224567 0.10224567 0.10224567
+ 0.1006018  0.1006018  0.1006018  0.09369312 0.09369312 0.09369312
+ 0.08752982 0.08752982 0.08752982 0.08259375 0.08259375 0.08259375]</t>
         </is>
       </c>
       <c r="E220" t="inlineStr"/>
@@ -5710,7 +5710,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>[1271391.6386005]</t>
+          <t>[1271281.66132225]</t>
         </is>
       </c>
       <c r="E227" t="inlineStr"/>
@@ -5733,7 +5733,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>[3123382.66878689]</t>
+          <t>[3123140.92507672]</t>
         </is>
       </c>
       <c r="E228" t="inlineStr"/>
@@ -5756,7 +5756,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>[36.04767429]</t>
+          <t>[36.05011418]</t>
         </is>
       </c>
       <c r="E229" t="inlineStr"/>
@@ -5779,7 +5779,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>[2.07326458e+09 2.07326458e+09 3.12794715e+07 0.00000000e+00
+          <t>[2.07345247e+09 2.07345247e+09 3.12768590e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -5803,7 +5803,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>[1331057.88767517]</t>
+          <t>[1331165.97109842]</t>
         </is>
       </c>
       <c r="E231" t="inlineStr"/>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>[3551873.58954871]</t>
+          <t>[3552111.19562842]</t>
         </is>
       </c>
       <c r="E232" t="inlineStr"/>
@@ -5915,9 +5915,9 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>[1.83676377 1.83676377 1.83676377 3.40231319 3.40231319 3.40231319
- 3.35207007 3.35207007 3.35207007 3.12142181 3.12142181 3.12142181
- 2.91610414 2.91610414 2.91610414 2.74976784 2.74976784 2.74976784]</t>
+          <t>[1.83680554 1.83680554 1.83680554 3.40185078 3.40185078 3.40185078
+ 3.34771288 3.34771288 3.34771288 3.11998944 3.11998944 3.11998944
+ 2.91656434 2.91656434 2.91656434 2.7534612  2.7534612  2.7534612 ]</t>
         </is>
       </c>
       <c r="E235" t="inlineStr"/>
@@ -5940,9 +5940,9 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952]</t>
         </is>
       </c>
       <c r="E236" t="inlineStr"/>
@@ -5965,9 +5965,9 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952]</t>
         </is>
       </c>
       <c r="E237" t="inlineStr"/>
@@ -5990,9 +5990,9 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411]</t>
         </is>
       </c>
       <c r="E238" t="inlineStr"/>
@@ -6015,9 +6015,9 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411]</t>
         </is>
       </c>
       <c r="E239" t="inlineStr"/>
@@ -6040,9 +6040,9 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>[45.41728    45.41728    45.41727999 83.33602078 83.33602079 83.3360208
- 82.13042053 82.13042052 82.13042052 76.58630203 76.58630203 76.58630203
- 71.63774363 71.63774363 71.63774363 67.61951737 67.61951737 67.61951736]</t>
+          <t>[45.41830148 45.41830148 45.41830148 83.32492866 83.32492866 83.32492866
+ 82.02583302 82.02583302 82.02583302 76.55182254 76.55182254 76.55182254
+ 71.64884942 71.64884942 71.64884942 67.70882823 67.70882823 67.70882823]</t>
         </is>
       </c>
       <c r="E240" t="inlineStr"/>
@@ -6237,8 +6237,8 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>[2.25504587 2.25504587 2.25504587 1.24769448 1.24769448 1.24769448
- 0.47150259 0.47150142 0.47150025 0.39473397 0.33826786 0.28180174]</t>
+          <t>[2.25604096 2.25604096 2.25604096 1.24727763 1.24727763 1.24727763
+ 0.47148028 0.47148028 0.47148028 0.39473641 0.33826931 0.28180221]</t>
         </is>
       </c>
       <c r="E247" t="inlineStr"/>
@@ -6261,8 +6261,8 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>[1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E248" t="inlineStr"/>
@@ -6285,8 +6285,8 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>[1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E249" t="inlineStr"/>
@@ -6309,8 +6309,8 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>[27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E250" t="inlineStr"/>
@@ -6333,8 +6333,8 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>[27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E251" t="inlineStr"/>
@@ -6357,8 +6357,8 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>[55.61975444 55.61975442 55.6197544  30.96080759 30.9608076  30.96080762
- 11.75446783 11.75438041 11.75429299  8.5731384   5.39521558  3.11930686]</t>
+          <t>[55.64396406 55.64396406 55.64396406 30.95054111 30.95054111 30.95054111
+ 11.75394248 11.75394248 11.75394248  8.57330591  5.39529059  3.11932561]</t>
         </is>
       </c>
       <c r="E252" t="inlineStr"/>
@@ -6453,8 +6453,8 @@
       <c r="D256" t="inlineStr">
         <is>
           <t>[10.         10.         10.         10.         10.         10.
- 10.          9.99997524  9.99995049  9.99992573  8.66661716  7.3333086
-  6.00000003]</t>
+ 10.         10.         10.         10.          8.66666752  7.33333503
+  6.00000255]</t>
         </is>
       </c>
       <c r="E256" t="inlineStr"/>
@@ -6477,8 +6477,8 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>[0.0675406  0.0675406  0.0675406  0.03725595 0.03725595 0.03725595
- 0.01404628 0.01404628 0.01404628 0.01259864 0.01259864 0.01259864]</t>
+          <t>[0.06757061 0.06757061 0.06757061 0.03724346 0.03724346 0.03724346
+ 0.0140456  0.0140456  0.0140456  0.01259863 0.01259863 0.01259863]</t>
         </is>
       </c>
       <c r="E257" t="inlineStr"/>
@@ -6585,7 +6585,7 @@
         <is>
           <t>[[ 2.91197623e+06]
  [-3.35507584e+03]
- [-1.97695612e+07]]</t>
+ [-1.97706224e+07]]</t>
         </is>
       </c>
       <c r="E261" t="inlineStr"/>
@@ -6608,8 +6608,8 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>[[-1.82360655e+05]
- [ 4.26821057e+08]
+          <t>[[-1.82361183e+05]
+ [ 4.26820404e+08]
  [ 6.48957511e+06]]</t>
         </is>
       </c>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>[1249999.99966499 1249999.99966499 2499999.99932998       0.
+          <t>[1249999.99999968 1249999.99999968 2499999.99999936       0.
        0.               0.        ]</t>
         </is>
       </c>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>[2313919.88767517]</t>
+          <t>[2314027.97109842]</t>
         </is>
       </c>
       <c r="E267" t="inlineStr"/>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>[-2.74163489e+00 -3.53965241e-02  9.91864249e+01]</t>
+          <t>[-2.74150683e+00 -3.53948708e-02  9.91792691e+01]</t>
         </is>
       </c>
       <c r="E268" t="inlineStr"/>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>[3.14386722e+10 3.12942480e+10 2.85379658e+08 2.02613158e+02
+          <t>[3.14380613e+10 3.12936371e+10 2.85382268e+08 2.02613158e+02
  1.08611945e+07 1.44041114e+05]</t>
         </is>
       </c>
@@ -6881,16 +6881,16 @@
           <t>[[      0.        ]
  [      0.        ]
  [      0.        ]
- [ -63274.56438251]
- [ -63567.52329466]
- [ -64449.93152488]
- [ -65932.48512269]
- [ -68033.35918549]
- [ -70778.7656079 ]
- [ -74203.80685615]
- [ -83285.51715675]
- [ -95797.25155505]
- [-112544.89762894]
+ [ -63274.56439359]
+ [ -63567.52330231]
+ [ -64449.93152909]
+ [ -65932.48512338]
+ [ -68033.35918758]
+ [ -70778.76561151]
+ [ -74203.80686143]
+ [ -83285.51716102]
+ [ -95797.25155807]
+ [-112544.89763027]
  [      0.        ]
  [      0.        ]
  [      0.        ]
@@ -6989,19 +6989,19 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>[[ -927.99815936]
- [-1070.12742471]
- [-1170.96499623]
- [-1251.15492773]
- [-1344.7463733 ]
- [-1422.65663252]
+          <t>[[ -927.99815941]
+ [-1070.12742489]
+ [-1170.96499657]
+ [-1251.15492825]
+ [-1344.74637368]
+ [-1422.65663272]
  [-1490.05546077]
- [-1526.70536514]
- [-1561.05280271]
- [-1593.42204527]
- [-1387.33212347]
- [-1189.05587167]
- [ -992.78219031]]</t>
+ [-1526.70959182]
+ [-1561.06149956]
+ [-1593.43543743]
+ [-1387.3406018 ]
+ [-1189.06011169]
+ [ -992.78259162]]</t>
         </is>
       </c>
       <c r="E275" t="inlineStr"/>
@@ -7024,24 +7024,24 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>[[-33863739.80132483]
- [-32458810.78678256]
- [-30740672.69993388]
- [-30202293.31443811]
- [-29662944.25102726]
- [-29121644.09487111]
- [-28583792.7195067 ]
- [-28041943.16216844]
- [-27495002.99396604]
- [-26439293.66241287]
- [-25347955.13371858]
- [-24208338.61119038]
- [-23279136.31635272]
- [-22535633.10125378]
- [-21792129.88615488]
- [-21441583.18977427]
- [-21091036.49339367]
- [-20740489.79701357]]</t>
+          <t>[[-33863690.88866773]
+ [-32458729.79287091]
+ [-30740559.6247678 ]
+ [-30202239.19855307]
+ [-29662949.09442247]
+ [-29121707.89754672]
+ [-28584411.95882652]
+ [-28043117.83813272]
+ [-27496733.10657578]
+ [-26441388.95865573]
+ [-25350415.6135943 ]
+ [-24211164.27469885]
+ [-23281844.63588943]
+ [-22538224.07681884]
+ [-21794603.51774818]
+ [-21443586.0090074 ]
+ [-21092568.50026697]
+ [-20741550.99152588]]</t>
         </is>
       </c>
       <c r="E276" t="inlineStr"/>
@@ -7064,24 +7064,24 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>[[ -3086085.81323177]
- [-10374388.86547915]
- [-13498928.84538622]
- [  2912284.79003139]
- [  2912312.34101361]
- [  2912340.37196493]
- [  2912364.69624453]
- [  2912394.2566323 ]
- [  2912424.82188857]
- [  2912920.36451624]
- [  2913061.43541644]
- [  2913220.56224855]
- [  2913165.78077624]
- [  2912943.11633556]
- [  2913017.02692222]
- [  2912493.31770458]
- [  2912511.13387485]
- [  2912528.73553031]]</t>
+          <t>[[ -3086154.97624959]
+ [-10374472.71212105]
+ [-13498863.57608701]
+ [  2912284.75458243]
+ [  2912312.30620923]
+ [  2912340.33781997]
+ [  2912364.32586176]
+ [  2912393.8931493 ]
+ [  2912424.46592084]
+ [  2912920.27729533]
+ [  2913061.36860698]
+ [  2913220.52258455]
+ [  2913166.24489117]
+ [  2912943.49949671]
+ [  2913017.41021343]
+ [  2912494.09599146]
+ [  2912511.91253024]
+ [  2912529.51454905]]</t>
         </is>
       </c>
       <c r="E277" t="inlineStr"/>
@@ -7104,24 +7104,24 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>[[ -560.1489822 ]
- [-2159.03251905]
- [-4236.0607079 ]
- [-3355.03222407]
- [-3355.0266181 ]
- [-3355.02059256]
- [-3355.01487829]
- [-3355.00787681]
- [-3355.00032166]
- [-3354.90907954]
- [-3354.87016243]
- [-3354.82367746]
- [-3354.8193481 ]
- [-3354.85338357]
- [-3354.82117502]
- [-3354.94384237]
- [-3354.93507694]
- [-3354.92607118]]</t>
+          <t>[[ -560.16401652]
+ [-2159.06126739]
+ [-4236.07156392]
+ [-3355.03222983]
+ [-3355.0266237 ]
+ [-3355.020598  ]
+ [-3355.01494316]
+ [-3355.00794003]
+ [-3355.00038301]
+ [-3354.90908266]
+ [-3354.87015984]
+ [-3354.82366688]
+ [-3354.81922512]
+ [-3354.85328368]
+ [-3354.82107499]
+ [-3354.94363808]
+ [-3354.93487244]
+ [-3354.92586648]]</t>
         </is>
       </c>
       <c r="E278" t="inlineStr"/>
@@ -7144,24 +7144,24 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>[[  -3427.06540599]
- [ -26916.32295169]
- [ -83454.47999688]
- [-102542.73264248]
- [-108125.35191884]
- [-113707.06577714]
- [-119287.867335  ]
- [-124867.71850547]
- [-130446.61160683]
- [-141601.18661971]
- [-152751.43684477]
- [-163897.44514248]
- [-175039.31668966]
- [-186176.46634685]
- [-197308.59348674]
- [-202873.02593154]
- [-208436.11925724]
- [-213997.87565573]]</t>
+          <t>[[  -3427.17392294]
+ [ -26916.78557248]
+ [ -83455.02725174]
+ [-102543.11964437]
+ [-108125.73898123]
+ [-113707.45273495]
+ [-119288.25462457]
+ [-124868.10441073]
+ [-130446.99435319]
+ [-141601.55801817]
+ [-152751.79398229]
+ [-163897.78494795]
+ [-175039.63655569]
+ [-186176.7672896 ]
+ [-197308.87642224]
+ [-202873.30017335]
+ [-208436.3876752 ]
+ [-213998.14118118]]</t>
         </is>
       </c>
       <c r="E279" t="inlineStr"/>
@@ -7184,24 +7184,24 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>[[2.63432389e+07]
- [1.74105677e+08]
- [4.22646099e+08]
- [5.01312414e+08]
- [4.96396477e+08]
- [4.91476750e+08]
- [4.86553414e+08]
- [4.81626668e+08]
- [4.76696746e+08]
- [4.66825893e+08]
- [4.56943413e+08]
- [4.47051387e+08]
- [4.37151335e+08]
- [4.27242918e+08]
- [4.17326020e+08]
- [4.12365557e+08]
- [4.07403203e+08]
- [4.02439103e+08]]</t>
+          <t>[[2.63440057e+07]
+ [1.74108038e+08]
+ [4.22647273e+08]
+ [5.01312368e+08]
+ [4.96396430e+08]
+ [4.91476702e+08]
+ [4.86553361e+08]
+ [4.81626602e+08]
+ [4.76696660e+08]
+ [4.66825754e+08]
+ [4.56943212e+08]
+ [4.47051115e+08]
+ [4.37150987e+08]
+ [4.27242499e+08]
+ [4.17325532e+08]
+ [4.12365040e+08]
+ [4.07402664e+08]
+ [4.02438547e+08]]</t>
         </is>
       </c>
       <c r="E280" t="inlineStr"/>
@@ -7224,24 +7224,24 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>[[ 925641.94365665]
- [2091197.09650497]
- [3798773.38633823]
- [6490314.59902542]
- [6490301.64647439]
- [6490288.67064628]
- [6490286.1492243 ]
- [6490273.01554051]
- [6490259.78427962]
- [6490296.03937005]
- [6490268.35532157]
- [6490239.7372107 ]
- [6490254.54922411]
- [6490228.46730628]
- [6490207.59795461]
- [6490223.72982414]
- [6490213.29514698]
- [6490202.86050342]]</t>
+          <t>[[ 925652.21769021]
+ [2091214.89246739]
+ [3798791.08352944]
+ [6490314.69680958]
+ [6490301.74391663]
+ [6490288.76774339]
+ [6490287.07628086]
+ [6490273.93908096]
+ [6490260.70417696]
+ [6490296.41578718]
+ [6490268.72860595]
+ [6490240.10693338]
+ [6490254.52126754]
+ [6490228.44017368]
+ [6490207.57082312]
+ [6490222.93327906]
+ [6490212.49860472]
+ [6490202.06396379]]</t>
         </is>
       </c>
       <c r="E281" t="inlineStr"/>
@@ -7297,8 +7297,8 @@
  10.         10.         10.         10.         10.         10.
  10.         10.         10.         10.         10.         10.
  10.         10.         10.         10.         10.         10.
- 10.          9.99997524  9.99995049  9.99992573  8.66661716  7.3333086
-  6.00000003]</t>
+ 10.         10.         10.         10.          8.66666752  7.33333503
+  6.00000255]</t>
         </is>
       </c>
       <c r="E283" t="inlineStr"/>
@@ -7321,11 +7321,11 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>[0.054943   0.054943   0.054943   0.10225972 0.10225972 0.10225972
- 0.10073409 0.10073409 0.10073409 0.09373654 0.09373654 0.09373654
- 0.08751588 0.08751588 0.08751588 0.08248204 0.08248204 0.08248204
- 0.0675406  0.0675406  0.0675406  0.03725595 0.03725595 0.03725595
- 0.01404628 0.01404628 0.01404628 0.01259864 0.01259864 0.01259864]</t>
+          <t>[0.05494426 0.05494426 0.05494426 0.10224567 0.10224567 0.10224567
+ 0.1006018  0.1006018  0.1006018  0.09369312 0.09369312 0.09369312
+ 0.08752982 0.08752982 0.08752982 0.08259375 0.08259375 0.08259375
+ 0.06757061 0.06757061 0.06757061 0.03724346 0.03724346 0.03724346
+ 0.0140456  0.0140456  0.0140456  0.01259863 0.01259863 0.01259863]</t>
         </is>
       </c>
       <c r="E284" t="inlineStr"/>
@@ -7473,11 +7473,11 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>[1.83676377 1.83676377 1.83676377 3.40231319 3.40231319 3.40231319
- 3.35207007 3.35207007 3.35207007 3.12142181 3.12142181 3.12142181
- 2.91610414 2.91610414 2.91610414 2.74976784 2.74976784 2.74976784
- 2.25504587 2.25504587 2.25504587 1.24769448 1.24769448 1.24769448
- 0.47150259 0.47150142 0.47150025 0.39473397 0.33826786 0.28180174]</t>
+          <t>[1.83680554 1.83680554 1.83680554 3.40185078 3.40185078 3.40185078
+ 3.34771288 3.34771288 3.34771288 3.11998944 3.11998944 3.11998944
+ 2.91656434 2.91656434 2.91656434 2.7534612  2.7534612  2.7534612
+ 2.25604096 2.25604096 2.25604096 1.24727763 1.24727763 1.24727763
+ 0.47148028 0.47148028 0.47148028 0.39473641 0.33826931 0.28180221]</t>
         </is>
       </c>
       <c r="E290" t="inlineStr"/>
@@ -7500,11 +7500,11 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756
- 1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952
+ 1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E291" t="inlineStr"/>
@@ -7527,11 +7527,11 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756
- 1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952
+ 1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E292" t="inlineStr"/>
@@ -7554,11 +7554,11 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868
- 27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411
+ 27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E293" t="inlineStr"/>
@@ -7581,11 +7581,11 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868
- 27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411
+ 27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E294" t="inlineStr"/>
@@ -7608,11 +7608,11 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>[45.41728    45.41728    45.41727999 83.33602078 83.33602079 83.3360208
- 82.13042053 82.13042052 82.13042052 76.58630203 76.58630203 76.58630203
- 71.63774363 71.63774363 71.63774363 67.61951737 67.61951737 67.61951736
- 55.61975444 55.61975442 55.6197544  30.96080759 30.9608076  30.96080762
- 11.75446783 11.75438041 11.75429299  8.5731384   5.39521558  3.11930686]</t>
+          <t>[45.41830148 45.41830148 45.41830148 83.32492866 83.32492866 83.32492866
+ 82.02583302 82.02583302 82.02583302 76.55182254 76.55182254 76.55182254
+ 71.64884942 71.64884942 71.64884942 67.70882823 67.70882823 67.70882823
+ 55.64396406 55.64396406 55.64396406 30.95054111 30.95054111 30.95054111
+ 11.75394248 11.75394248 11.75394248  8.57330591  5.39529059  3.11932561]</t>
         </is>
       </c>
       <c r="E295" t="inlineStr"/>
@@ -7635,36 +7635,36 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>[[-3.38637398e+07]
- [-3.24588108e+07]
- [-3.07406727e+07]
- [-3.02022933e+07]
- [-2.96629443e+07]
- [-2.91216441e+07]
- [-2.85837927e+07]
- [-2.80419432e+07]
- [-2.74950030e+07]
- [-2.64392937e+07]
- [-2.53479551e+07]
- [-2.42083386e+07]
- [-2.32791363e+07]
- [-2.25356331e+07]
- [-2.17921299e+07]
- [-2.14415832e+07]
- [-2.10910365e+07]
- [-2.07404898e+07]
- [-1.76721640e+07]
- [-1.55780768e+07]
- [-1.34825379e+07]
- [-1.18161028e+07]
- [-1.01481843e+07]
- [-8.47880185e+06]
- [-8.09072522e+06]
- [-7.70211664e+06]
- [-7.31314534e+06]
- [-7.00649092e+06]
- [-6.74237634e+06]
- [ 3.75439413e-09]]</t>
+          <t>[[-3.38636909e+07]
+ [-3.24587298e+07]
+ [-3.07405596e+07]
+ [-3.02022392e+07]
+ [-2.96629491e+07]
+ [-2.91217079e+07]
+ [-2.85844120e+07]
+ [-2.80431178e+07]
+ [-2.74967331e+07]
+ [-2.64413890e+07]
+ [-2.53504156e+07]
+ [-2.42111643e+07]
+ [-2.32818446e+07]
+ [-2.25382241e+07]
+ [-2.17946035e+07]
+ [-2.14435860e+07]
+ [-2.10925685e+07]
+ [-2.07415510e+07]
+ [-1.76723062e+07]
+ [-1.55773000e+07]
+ [-1.34808420e+07]
+ [-1.18149567e+07]
+ [-1.01475880e+07]
+ [-8.47875525e+06]
+ [-8.09069629e+06]
+ [-7.70210441e+06]
+ [-7.31314885e+06]
+ [-7.00649251e+06]
+ [-6.74237674e+06]
+ [-2.41561793e-09]]</t>
         </is>
       </c>
       <c r="E296" t="inlineStr"/>
@@ -7687,36 +7687,36 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>[[-3.08608581e+06]
- [-1.03743889e+07]
- [-1.34989288e+07]
- [ 2.91228479e+06]
- [ 2.91231234e+06]
- [ 2.91234037e+06]
- [ 2.91236470e+06]
- [ 2.91239426e+06]
- [ 2.91242482e+06]
- [ 2.91292036e+06]
- [ 2.91306144e+06]
- [ 2.91322056e+06]
- [ 2.91316578e+06]
- [ 2.91294312e+06]
- [ 2.91301703e+06]
- [ 2.91249332e+06]
- [ 2.91251113e+06]
- [ 2.91252874e+06]
- [ 2.91576355e+06]
- [ 2.91661077e+06]
- [ 2.91736537e+06]
- [ 2.91720256e+06]
- [ 2.91833381e+06]
- [ 2.91922658e+06]
- [ 2.91387308e+06]
+          <t>[[-3.08615498e+06]
+ [-1.03744727e+07]
+ [-1.34988636e+07]
+ [ 2.91228475e+06]
+ [ 2.91231231e+06]
+ [ 2.91234034e+06]
+ [ 2.91236433e+06]
+ [ 2.91239389e+06]
+ [ 2.91242447e+06]
+ [ 2.91292028e+06]
+ [ 2.91306137e+06]
+ [ 2.91322052e+06]
+ [ 2.91316624e+06]
+ [ 2.91294350e+06]
+ [ 2.91301741e+06]
+ [ 2.91249410e+06]
+ [ 2.91251191e+06]
+ [ 2.91252951e+06]
+ [ 2.91576520e+06]
+ [ 2.91661242e+06]
+ [ 2.91736702e+06]
+ [ 2.91720038e+06]
+ [ 2.91833164e+06]
+ [ 2.91922441e+06]
+ [ 2.91387307e+06]
  [ 2.91406083e+06]
- [ 2.91419470e+06]
- [ 2.91379896e+06]
- [ 2.91358078e+06]
- [ 1.31558268e+03]]</t>
+ [ 2.91419471e+06]
+ [ 2.91379904e+06]
+ [ 2.91358085e+06]
+ [ 1.31563810e+03]]</t>
         </is>
       </c>
       <c r="E297" t="inlineStr"/>
@@ -7739,36 +7739,36 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>[[ -560.1489822 ]
- [-2159.03251905]
- [-4236.0607079 ]
- [-3355.03222407]
- [-3355.0266181 ]
- [-3355.02059256]
- [-3355.01487829]
- [-3355.00787681]
- [-3355.00032166]
- [-3354.90907954]
- [-3354.87016243]
- [-3354.82367746]
- [-3354.8193481 ]
- [-3354.85338357]
- [-3354.82117502]
- [-3354.94384237]
- [-3354.93507694]
- [-3354.92607118]
- [-3353.90639329]
- [-3353.32416013]
- [-3352.65341641]
- [-3352.06182566]
- [-3350.24068341]
- [-3348.15262212]
- [-3352.7815077 ]
- [-3351.85699315]
- [-3350.87494886]
- [-3350.83621269]
- [-3350.19334229]
- [    4.74684048]]</t>
+          <t>[[ -560.16401652]
+ [-2159.06126739]
+ [-4236.07156392]
+ [-3355.03222983]
+ [-3355.0266237 ]
+ [-3355.020598  ]
+ [-3355.01494316]
+ [-3355.00794003]
+ [-3355.00038301]
+ [-3354.90908266]
+ [-3354.87015984]
+ [-3354.82366688]
+ [-3354.81922512]
+ [-3354.85328368]
+ [-3354.82107499]
+ [-3354.94363808]
+ [-3354.93487244]
+ [-3354.92586648]
+ [-3353.90602718]
+ [-3353.32379186]
+ [-3352.65304542]
+ [-3352.06325097]
+ [-3350.24210199]
+ [-3348.15403191]
+ [-3352.78129943]
+ [-3351.8567796 ]
+ [-3350.87473307]
+ [-3350.83587903]
+ [-3350.19307457]
+ [    4.74704529]]</t>
         </is>
       </c>
       <c r="E298" t="inlineStr"/>
@@ -7791,36 +7791,36 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>[[-3.42706541e+03]
- [-2.69163230e+04]
- [-8.34544800e+04]
- [-1.02542733e+05]
- [-1.08125352e+05]
- [-1.13707066e+05]
- [-1.19287867e+05]
- [-1.24867719e+05]
- [-1.30446612e+05]
- [-1.41601187e+05]
- [-1.52751437e+05]
- [-1.63897445e+05]
- [-1.75039317e+05]
- [-1.86176466e+05]
- [-1.97308593e+05]
- [-2.02873026e+05]
- [-2.08436119e+05]
- [-2.13997876e+05]
- [-2.54231113e+05]
- [-2.94374456e+05]
- [-3.34439945e+05]
- [-3.91457689e+05]
- [-4.48133769e+05]
- [-5.04539806e+05]
- [-5.38214575e+05]
- [-5.71542576e+05]
- [-6.04536130e+05]
- [-6.34984081e+05]
- [-6.64887307e+05]
- [-1.19850988e-04]]</t>
+          <t>[[-3.42717392e+03]
+ [-2.69167856e+04]
+ [-8.34550273e+04]
+ [-1.02543120e+05]
+ [-1.08125739e+05]
+ [-1.13707453e+05]
+ [-1.19288255e+05]
+ [-1.24868104e+05]
+ [-1.30446994e+05]
+ [-1.41601558e+05]
+ [-1.52751794e+05]
+ [-1.63897785e+05]
+ [-1.75039637e+05]
+ [-1.86176767e+05]
+ [-1.97308876e+05]
+ [-2.02873300e+05]
+ [-2.08436388e+05]
+ [-2.13998141e+05]
+ [-2.54231399e+05]
+ [-2.94374820e+05]
+ [-3.34440455e+05]
+ [-3.91458425e+05]
+ [-4.48134577e+05]
+ [-5.04540517e+05]
+ [-5.38215149e+05]
+ [-5.71543004e+05]
+ [-6.04536403e+05]
+ [-6.34984211e+05]
+ [-6.64887311e+05]
+ [-1.19856604e-04]]</t>
         </is>
       </c>
       <c r="E299" t="inlineStr"/>
@@ -7843,36 +7843,36 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>[[ 2.63432389e+07]
- [ 1.74105677e+08]
- [ 4.22646099e+08]
- [ 5.01312414e+08]
- [ 4.96396477e+08]
- [ 4.91476750e+08]
- [ 4.86553414e+08]
- [ 4.81626668e+08]
- [ 4.76696746e+08]
- [ 4.66825893e+08]
- [ 4.56943413e+08]
- [ 4.47051387e+08]
- [ 4.37151335e+08]
- [ 4.27242918e+08]
- [ 4.17326020e+08]
- [ 4.12365557e+08]
- [ 4.07403203e+08]
- [ 4.02439103e+08]
- [ 3.66422437e+08]
- [ 3.30326665e+08]
- [ 2.94207961e+08]
- [ 2.42534673e+08]
- [ 1.90764894e+08]
- [ 1.39028386e+08]
- [ 1.08040213e+08]
- [ 7.70125221e+07]
- [ 4.59739259e+07]
- [ 1.70135072e+07]
- [-1.19282330e+07]
- [ 3.32160984e-02]]</t>
+          <t>[[ 2.63440057e+07]
+ [ 1.74108038e+08]
+ [ 4.22647273e+08]
+ [ 5.01312368e+08]
+ [ 4.96396430e+08]
+ [ 4.91476702e+08]
+ [ 4.86553361e+08]
+ [ 4.81626602e+08]
+ [ 4.76696660e+08]
+ [ 4.66825754e+08]
+ [ 4.56943212e+08]
+ [ 4.47051115e+08]
+ [ 4.37150987e+08]
+ [ 4.27242499e+08]
+ [ 4.17325532e+08]
+ [ 4.12365040e+08]
+ [ 4.07402664e+08]
+ [ 4.02438547e+08]
+ [ 3.66421840e+08]
+ [ 3.30326140e+08]
+ [ 2.94207612e+08]
+ [ 2.42534632e+08]
+ [ 1.90765023e+08]
+ [ 1.39028559e+08]
+ [ 1.08040354e+08]
+ [ 7.70126274e+07]
+ [ 4.59739939e+07]
+ [ 1.70135408e+07]
+ [-1.19282319e+07]
+ [ 3.32183813e-02]]</t>
         </is>
       </c>
       <c r="E300" t="inlineStr"/>
@@ -7895,36 +7895,36 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>[[9.25641944e+05]
- [2.09119710e+06]
- [3.79877339e+06]
- [6.49031460e+06]
- [6.49030165e+06]
- [6.49028867e+06]
- [6.49028615e+06]
- [6.49027302e+06]
- [6.49025978e+06]
- [6.49029604e+06]
- [6.49026836e+06]
- [6.49023974e+06]
- [6.49025455e+06]
- [6.49022847e+06]
- [6.49020760e+06]
- [6.49022373e+06]
- [6.49021330e+06]
- [6.49020286e+06]
- [6.49029228e+06]
- [6.49021650e+06]
- [6.49014049e+06]
- [6.49045954e+06]
- [6.49035022e+06]
- [6.49024079e+06]
- [6.49104706e+06]
- [6.49097967e+06]
- [6.49091220e+06]
- [6.49109162e+06]
- [6.49127060e+06]
- [2.77713178e-09]]</t>
+          <t>[[ 9.25652218e+05]
+ [ 2.09121489e+06]
+ [ 3.79879108e+06]
+ [ 6.49031470e+06]
+ [ 6.49030174e+06]
+ [ 6.49028877e+06]
+ [ 6.49028708e+06]
+ [ 6.49027394e+06]
+ [ 6.49026070e+06]
+ [ 6.49029642e+06]
+ [ 6.49026873e+06]
+ [ 6.49024011e+06]
+ [ 6.49025452e+06]
+ [ 6.49022844e+06]
+ [ 6.49020757e+06]
+ [ 6.49022293e+06]
+ [ 6.49021250e+06]
+ [ 6.49020206e+06]
+ [ 6.49029200e+06]
+ [ 6.49021622e+06]
+ [ 6.49014021e+06]
+ [ 6.49045973e+06]
+ [ 6.49035040e+06]
+ [ 6.49024098e+06]
+ [ 6.49104712e+06]
+ [ 6.49097973e+06]
+ [ 6.49091225e+06]
+ [ 6.49109161e+06]
+ [ 6.49127060e+06]
+ [-2.77714871e-09]]</t>
         </is>
       </c>
       <c r="E301" t="inlineStr"/>
@@ -8621,7 +8621,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>[3551873.58954871]</t>
+          <t>[3552111.19562842]</t>
         </is>
       </c>
       <c r="E330" t="inlineStr"/>
@@ -8644,7 +8644,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>[1331057.88767517]</t>
+          <t>[1331165.97109842]</t>
         </is>
       </c>
       <c r="E331" t="inlineStr"/>
@@ -8667,7 +8667,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>[4496873.58954871]</t>
+          <t>[4497111.19562842]</t>
         </is>
       </c>
       <c r="E332" t="inlineStr"/>
@@ -8690,7 +8690,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>[299.79157264]</t>
+          <t>[299.80741304]</t>
         </is>
       </c>
       <c r="E333" t="inlineStr"/>
@@ -8713,7 +8713,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>[1331057.88767517]</t>
+          <t>[1331165.97109842]</t>
         </is>
       </c>
       <c r="E334" t="inlineStr"/>
@@ -8782,7 +8782,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>[3551873.58954871]</t>
+          <t>[3552111.19562842]</t>
         </is>
       </c>
       <c r="E337" t="inlineStr"/>
@@ -8805,7 +8805,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>[3551873.58954871]</t>
+          <t>[3552111.19562842]</t>
         </is>
       </c>
       <c r="E338" t="inlineStr"/>
@@ -8828,9 +8828,9 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>[ 927.99815936 1070.12742471 1170.96499623 1251.15492773 1344.7463733
- 1422.65663252 1490.05546077 1526.70536514 1561.05280271 1593.42204527
- 1387.33212347 1189.05587167  992.78219031]</t>
+          <t>[ 927.99815941 1070.12742489 1170.96499657 1251.15492825 1344.74637368
+ 1422.65663272 1490.05546077 1526.70959182 1561.06149956 1593.43543743
+ 1387.3406018  1189.06011169  992.78259162]</t>
         </is>
       </c>
       <c r="E339" t="inlineStr"/>
@@ -9046,8 +9046,8 @@
       <c r="D348" t="inlineStr">
         <is>
           <t>[10.         10.         10.         10.         10.         10.
- 10.          9.99997524  9.99995049  9.99992573  8.66661716  7.3333086
-  6.00000003]</t>
+ 10.         10.         10.         10.          8.66666752  7.33333503
+  6.00000255]</t>
         </is>
       </c>
       <c r="E348" t="inlineStr"/>
@@ -9141,9 +9141,9 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>[ 927.99815936 1070.12742471 1170.96499623 1251.15492773 1344.7463733
- 1422.65663252 1490.05546077 1526.70536514 1561.05280271 1593.42204527
- 1387.33212347 1189.05587167  992.78219031]</t>
+          <t>[ 927.99815941 1070.12742489 1170.96499657 1251.15492825 1344.74637368
+ 1422.65663272 1490.05546077 1526.70959182 1561.06149956 1593.43543743
+ 1387.3406018  1189.06011169  992.78259162]</t>
         </is>
       </c>
       <c r="E352" t="inlineStr"/>
@@ -9283,10 +9283,10 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>[ -927.99815936 -1070.12742471 -1170.96499623 -1251.15492773
- -1344.7463733  -1422.65663252 -1490.05546077 -1526.70536514
- -1561.05280271 -1593.42204527 -1387.33212347 -1189.05587167
-  -992.78219031]</t>
+          <t>[ -927.99815941 -1070.12742489 -1170.96499657 -1251.15492825
+ -1344.74637368 -1422.65663272 -1490.05546077 -1526.70959182
+ -1561.06149956 -1593.43543743 -1387.3406018  -1189.06011169
+  -992.78259162]</t>
         </is>
       </c>
       <c r="E358" t="inlineStr"/>
@@ -9334,7 +9334,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          9.99992573  6.00000003]</t>
+          <t>[10.         10.         10.         10.          6.00000255]</t>
         </is>
       </c>
       <c r="E360" t="inlineStr"/>
@@ -9357,7 +9357,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>[0.0675406  0.03725595 0.01404628 0.01259864]</t>
+          <t>[0.06757061 0.03724346 0.0140456  0.01259863]</t>
         </is>
       </c>
       <c r="E361" t="inlineStr"/>
@@ -9422,7 +9422,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          9.99992573  6.00000003]</t>
+          <t>[10.         10.         10.         10.          6.00000255]</t>
         </is>
       </c>
       <c r="E364" t="inlineStr"/>
@@ -9445,7 +9445,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>[0.0675406  0.03725595 0.01404628 0.01259864]</t>
+          <t>[0.06757061 0.03724346 0.0140456  0.01259863]</t>
         </is>
       </c>
       <c r="E365" t="inlineStr"/>
@@ -9681,8 +9681,8 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>[0.0675406  0.0675406  0.0675406  0.03725595 0.03725595 0.03725595
- 0.01404628 0.01404628 0.01404628 0.01259864 0.01259864 0.01259864]</t>
+          <t>[0.06757061 0.06757061 0.06757061 0.03724346 0.03724346 0.03724346
+ 0.0140456  0.0140456  0.0140456  0.01259863 0.01259863 0.01259863]</t>
         </is>
       </c>
       <c r="E375" t="inlineStr"/>
@@ -9865,8 +9865,8 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>[2.25504587 2.25504587 2.25504587 1.24769448 1.24769448 1.24769448
- 0.47150259 0.47150142 0.47150025 0.39473397 0.33826786 0.28180174]</t>
+          <t>[2.25604096 2.25604096 2.25604096 1.24727763 1.24727763 1.24727763
+ 0.47148028 0.47148028 0.47148028 0.39473641 0.33826931 0.28180221]</t>
         </is>
       </c>
       <c r="E383" t="inlineStr"/>
@@ -9889,8 +9889,8 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>[1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E384" t="inlineStr"/>
@@ -9913,8 +9913,8 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>[1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E385" t="inlineStr"/>
@@ -9937,8 +9937,8 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>[27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E386" t="inlineStr"/>
@@ -9961,8 +9961,8 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>[27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E387" t="inlineStr"/>
@@ -9985,8 +9985,8 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>[55.61975444 55.61975442 55.6197544  30.96080759 30.9608076  30.96080762
- 11.75446783 11.75438041 11.75429299  8.5731384   5.39521558  3.11930686]</t>
+          <t>[55.64396406 55.64396406 55.64396406 30.95054111 30.95054111 30.95054111
+ 11.75394248 11.75394248 11.75394248  8.57330591  5.39529059  3.11932561]</t>
         </is>
       </c>
       <c r="E388" t="inlineStr"/>
@@ -10080,18 +10080,18 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>[[-17675474.04604535]
- [-15579935.09648651]
- [-13483314.45143045]
- [-11815395.94933672]
- [-10146013.48436328]
- [ -8475390.63871807]
- [ -8086781.11118934]
- [ -7697808.89734239]
- [ -7308495.89839982]
- [ -7002671.90023286]
- [ -6740490.2916013 ]
- [ -6521904.15      ]]</t>
+          <t>[[-17675616.2423275 ]
+ [-15579158.26477832]
+ [-13481618.59173192]
+ [-11814249.85498947]
+ [-10145417.15536732]
+ [ -8475344.07507338]
+ [ -8086752.18721936]
+ [ -7697796.62921059]
+ [ -7308499.32078923]
+ [ -7002673.41537894]
+ [ -6740490.66057829]
+ [ -6521904.14999999]]</t>
         </is>
       </c>
       <c r="E392" t="inlineStr"/>
@@ -10114,18 +10114,18 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>[[2912478.11046093]
- [2913368.97104382]
- [2914180.04028183]
- [2914756.09703146]
- [2916012.11928344]
- [2917031.38834743]
- [2913403.03363594]
- [2913637.90766991]
- [2913820.22876347]
- [2913544.10820134]
- [2913407.77523025]
- [2913212.87537518]]</t>
+          <t>[[2912478.11130552]
+ [2913368.97325693]
+ [2914180.04351811]
+ [2914754.54334205]
+ [2916010.56784803]
+ [2917029.83997802]
+ [2913403.03274234]
+ [2913637.91025541]
+ [2913820.23451225]
+ [2913544.18065396]
+ [2913407.83396474]
+ [2913212.92091163]]</t>
         </is>
       </c>
       <c r="E393" t="inlineStr"/>
@@ -10148,18 +10148,18 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>[[-3354.88807516]
- [-3354.38119436]
- [-3353.78198272]
- [-3353.05800832]
- [-3351.37882345]
- [-3349.43236305]
- [-3353.1192241 ]
- [-3352.24685734]
- [-3351.3156365 ]
- [-3351.23778429]
- [-3350.62488113]
- [-3349.66084702]]</t>
+          <t>[[-3354.88807363]
+ [-3354.38119   ]
+ [-3353.78197533]
+ [-3353.05901088]
+ [-3351.3798183 ]
+ [-3349.43334846]
+ [-3353.11900603]
+ [-3352.2466345 ]
+ [-3351.31541167]
+ [-3351.23746102]
+ [-3350.62462325]
+ [-3349.66065387]]</t>
         </is>
       </c>
       <c r="E394" t="inlineStr"/>
@@ -10182,18 +10182,18 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>[[-222818.48080534]
- [-263177.27897981]
- [-303445.42093956]
- [-360741.47095881]
- [-417696.52490672]
- [-474372.03354204]
- [-508201.33172902]
- [-541699.01683295]
- [-574875.34008509]
- [-605506.65431162]
- [-635614.79310258]
- [-664796.34298229]]</t>
+          <t>[[-222819.02440323]
+ [-263177.88259038]
+ [-303446.13652196]
+ [-360742.35133171]
+ [-417697.43838069]
+ [-474372.83378987]
+ [-508201.9983294 ]
+ [-541699.53980934]
+ [-574875.71153478]
+ [-605506.88701382]
+ [-635614.90256503]
+ [-664796.34297475]]</t>
         </is>
       </c>
       <c r="E395" t="inlineStr"/>
@@ -10216,17 +10216,17 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>[[ 3.91556225e+08]
- [ 3.56121148e+08]
- [ 3.20574315e+08]
- [ 2.69584450e+08]
- [ 2.18382917e+08]
- [ 1.67107693e+08]
- [ 1.36333111e+08]
- [ 1.05488617e+08]
- [ 7.46045244e+07]
- [ 4.57608196e+07]
- [ 1.69025028e+07]
+          <t>[[ 3.91555616e+08]
+ [ 3.56120660e+08]
+ [ 3.20574020e+08]
+ [ 2.69584431e+08]
+ [ 2.18383047e+08]
+ [ 1.67107861e+08]
+ [ 1.36333254e+08]
+ [ 1.05488731e+08]
+ [ 7.46046067e+07]
+ [ 4.57608727e+07]
+ [ 1.69025286e+07]
  [-1.19535912e+07]]</t>
         </is>
       </c>
@@ -10250,18 +10250,18 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>[[6490292.62802801]
- [6490216.61756634]
- [6490140.55618992]
- [6490459.59550754]
- [6490350.16947062]
- [6490240.65108298]
- [6491046.46406648]
- [6490978.98919581]
- [6490911.45234288]
- [6491090.65218141]
- [6491269.68007644]
- [6491533.15181504]]</t>
+          <t>[[6490292.35003889]
+ [6490216.3397639 ]
+ [6490140.2785974 ]
+ [6490459.77987847]
+ [6490350.35334112]
+ [6490240.83442098]
+ [6491046.52567378]
+ [6490979.04713555]
+ [6490911.50685135]
+ [6491090.64352078]
+ [6491269.67314822]
+ [6491533.14849952]]</t>
         </is>
       </c>
       <c r="E397" t="inlineStr"/>
@@ -10435,19 +10435,19 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>[[ -927.99815936]
- [-1070.12742471]
- [-1170.96499623]
- [-1251.15492773]
- [-1344.7463733 ]
- [-1422.65663252]
+          <t>[[ -927.99815941]
+ [-1070.12742489]
+ [-1170.96499657]
+ [-1251.15492825]
+ [-1344.74637368]
+ [-1422.65663272]
  [-1490.05546077]
- [-1526.70536514]
- [-1561.05280271]
- [-1593.42204527]
- [-1387.33212347]
- [-1189.05587167]
- [ -992.78219031]]</t>
+ [-1526.70959182]
+ [-1561.06149956]
+ [-1593.43543743]
+ [-1387.3406018 ]
+ [-1189.06011169]
+ [ -992.78259162]]</t>
         </is>
       </c>
       <c r="E403" t="inlineStr"/>
@@ -10470,7 +10470,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>[1331057.88767517]</t>
+          <t>[1331165.97109842]</t>
         </is>
       </c>
       <c r="E404" t="inlineStr"/>
@@ -10493,7 +10493,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>[48.6173439]</t>
+          <t>[48.60901061]</t>
         </is>
       </c>
       <c r="E405" t="inlineStr"/>
@@ -10516,7 +10516,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>[4.92116776e+09 4.92116776e+09 3.23459422e+07 0.00000000e+00
+          <t>[4.92055682e+09 4.92055682e+09 3.23485519e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -10571,10 +10571,10 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          63274.56438251
-  63567.52329466  64449.93152488  65932.48512269  68033.35918549
-  70778.7656079   74203.80685615  83285.51715675  95797.25155505
- 112544.89762894      0.              0.              0.
+          <t>[     0.              0.              0.          63274.56439359
+  63567.52330231  64449.93152909  65932.48512338  68033.35918758
+  70778.76561151  74203.80686143  83285.51716102  95797.25155807
+ 112544.89763027      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -10825,10 +10825,10 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          63274.56438251
-  63567.52329466  64449.93152488  65932.48512269  68033.35918549
-  70778.7656079   74203.80685615  83285.51715675  95797.25155505
- 112544.89762894      0.              0.              0.
+          <t>[     0.              0.              0.          63274.56439359
+  63567.52330231  64449.93152909  65932.48512338  68033.35918758
+  70778.76561151  74203.80686143  83285.51716102  95797.25155807
+ 112544.89763027      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -11210,10 +11210,10 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -63274.56438251
-  -63567.52329466  -64449.93152488  -65932.48512269  -68033.35918549
-  -70778.7656079   -74203.80685615  -83285.51715675  -95797.25155505
- -112544.89762894       0.               0.               0.
+          <t>[      0.               0.               0.          -63274.56439359
+  -63567.52330231  -64449.93152909  -65932.48512338  -68033.35918758
+  -70778.76561151  -74203.80686143  -83285.51716102  -95797.25155807
+ -112544.89763027       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -11260,8 +11260,8 @@
       <c r="C436" t="inlineStr"/>
       <c r="D436" t="inlineStr">
         <is>
-          <t>[182.00680367  97.79021836  99.27126416 106.68197905 114.26497406
- 121.23851777]</t>
+          <t>[182.00264153  97.80364951  99.40179808 106.73142404 114.24678372
+ 121.07453023]</t>
         </is>
       </c>
       <c r="E436" t="inlineStr"/>
@@ -11318,7 +11318,7 @@
       <c r="C439" t="inlineStr"/>
       <c r="D439" t="inlineStr">
         <is>
-          <t>[1.86119641 0.98508082 0.93053452 0.93363675 0.94248079]</t>
+          <t>[1.86089826 0.98392234 0.93132645 0.93421819 0.94360708]</t>
         </is>
       </c>
       <c r="E439" t="inlineStr"/>
@@ -11408,7 +11408,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>[3926.99081665]</t>
+          <t>[3926.99081699]</t>
         </is>
       </c>
       <c r="E443" t="inlineStr"/>
@@ -11431,7 +11431,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>[39472102.05137084]</t>
+          <t>[39472102.05479642]</t>
         </is>
       </c>
       <c r="E444" t="inlineStr"/>
@@ -11450,7 +11450,7 @@
       <c r="C445" t="inlineStr"/>
       <c r="D445" t="inlineStr">
         <is>
-          <t>[3.]</t>
+          <t>[2.]</t>
         </is>
       </c>
       <c r="E445" t="inlineStr"/>
@@ -11496,7 +11496,7 @@
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>[490.87385211]</t>
+          <t>[490.87385212]</t>
         </is>
       </c>
       <c r="E447" t="inlineStr"/>
@@ -11519,7 +11519,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>[490.87385211]</t>
+          <t>[490.87385212]</t>
         </is>
       </c>
       <c r="E448" t="inlineStr"/>
@@ -11870,8 +11870,8 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>[14326.75739622 26538.04284428 26146.1465516  24347.09011645
- 22745.6122928  21448.1891284 ]</t>
+          <t>[14327.08321983 26534.43608568 26112.16050189 24335.91762866
+ 22749.20186459 21476.99737138]</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
@@ -11898,8 +11898,8 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>[177127.39198322 325010.48108951 320308.64004723 298686.57791394
- 279387.20016329 263716.11773682]</t>
+          <t>[177131.37577974 324967.22178745 319900.74876046 298552.10790767
+ 279430.51272725 264064.43009258]</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
@@ -11926,8 +11926,8 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>[177127.39198322 325010.48108951 320308.64004723 298686.57791394
- 279387.20016329 263716.11773682]</t>
+          <t>[177131.37577974 324967.22178745 319900.74876046 298552.10790767
+ 279430.51272725 264064.43009258]</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -11954,8 +11954,8 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>[4.24460561e+12 7.78841316e+12 7.67574024e+12 7.15759832e+12
- 6.69511623e+12 6.31958106e+12]</t>
+          <t>[4.24470107e+12 7.78737651e+12 7.66596570e+12 7.15437594e+12
+ 6.69615415e+12 6.32792787e+12]</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -11982,8 +11982,8 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>[4.24460561e+12 7.78841316e+12 7.67574024e+12 7.15759832e+12
- 6.69511623e+12 6.31958106e+12]</t>
+          <t>[4.24470107e+12 7.78737651e+12 7.66596570e+12 7.15437594e+12
+ 6.69615415e+12 6.32792787e+12]</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -12010,8 +12010,8 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>[3.36597225e+12 6.17621163e+12 6.08686201e+12 5.67597547e+12
- 5.30922717e+12 5.01142778e+12]</t>
+          <t>[3.36604795e+12 6.17538957e+12 6.07911080e+12 5.67342012e+12
+ 5.31005024e+12 5.01804680e+12]</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -12038,8 +12038,8 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>[3.43320331e+11 6.35946390e+11 6.26555153e+11 5.83443329e+11
- 5.45066194e+11 5.13975297e+11]</t>
+          <t>[3.43328139e+11 6.35859959e+11 6.25740726e+11 5.83175596e+11
+ 5.45152213e+11 5.14665645e+11]</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
@@ -12147,12 +12147,12 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>[[0.         0.         0.58254633 0.23559315 0.23559315 0.        ]
- [0.         0.         0.31449192 0.12839586 0.12839586 0.        ]
- [0.         0.         0.31920574 0.13028059 0.13028059 0.        ]
- [0.         0.         0.3427925  0.13971167 0.13971167 0.        ]
- [0.         0.         0.36692791 0.1493626  0.1493626  0.        ]
- [0.         0.         0.38912376 0.15823834 0.15823834 0.        ]]</t>
+          <t>[[0.         0.         0.58253309 0.23558785 0.23558785 0.        ]
+ [0.         0.         0.31453467 0.12841295 0.12841295 0.        ]
+ [0.         0.         0.3196212  0.13044671 0.13044671 0.        ]
+ [0.         0.         0.34294988 0.1397746  0.1397746  0.        ]
+ [0.         0.         0.36687001 0.14933945 0.14933945 0.        ]
+ [0.         0.         0.38860181 0.15802961 0.15802961 0.        ]]</t>
         </is>
       </c>
       <c r="E473" t="inlineStr"/>
@@ -12175,12 +12175,12 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>[[0.95705046 0.95705046 0.         0.         0.         0.11779657]
- [0.51552741 0.51552741 0.         0.         0.         0.06419793]
- [0.52329258 0.52329258 0.         0.         0.         0.0651403 ]
- [0.56214676 0.56214676 0.         0.         0.         0.06985583]
- [0.60190356 0.60190356 0.         0.         0.         0.0746813 ]
- [0.63846459 0.63846459 0.         0.         0.         0.07911917]]</t>
+          <t>[[0.95702864 0.95702864 0.         0.         0.         0.11779393]
+ [0.51559783 0.51559783 0.         0.         0.         0.06420648]
+ [0.52397697 0.52397697 0.         0.         0.         0.06522335]
+ [0.562406   0.562406   0.         0.         0.         0.0698873 ]
+ [0.60180819 0.60180819 0.         0.         0.         0.07466973]
+ [0.63760484 0.63760484 0.         0.         0.         0.07901481]]</t>
         </is>
       </c>
       <c r="E474" t="inlineStr"/>
@@ -12203,7 +12203,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>[1083.37709107]</t>
+          <t>[1083.34939261]</t>
         </is>
       </c>
       <c r="E475" t="inlineStr"/>
@@ -12226,7 +12226,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>[3123382.66878689]</t>
+          <t>[3123140.92507672]</t>
         </is>
       </c>
       <c r="E476" t="inlineStr"/>
@@ -12249,7 +12249,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>[1271391.6386005]</t>
+          <t>[1271281.66132225]</t>
         </is>
       </c>
       <c r="E477" t="inlineStr"/>
@@ -12272,7 +12272,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>[36.04767429]</t>
+          <t>[36.05011418]</t>
         </is>
       </c>
       <c r="E478" t="inlineStr"/>
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>[2.07326458e+09 2.07326458e+09 3.12794715e+07 0.00000000e+00
+          <t>[2.07345247e+09 2.07345247e+09 3.12768590e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12342,9 +12342,9 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>[0.05878901 0.05878901 0.05878901 0.1094179  0.1094179  0.1094179
- 0.10778547 0.10778547 0.10778547 0.1002981  0.1002981  0.1002981
- 0.09364199 0.09364199 0.09364199 0.08825578 0.08825578 0.08825578]</t>
+          <t>[0.05879036 0.05879036 0.05879036 0.10940287 0.10940287 0.10940287
+ 0.10764393 0.10764393 0.10764393 0.10025164 0.10025164 0.10025164
+ 0.0936569  0.0936569  0.0936569  0.08837532 0.08837532 0.08837532]</t>
         </is>
       </c>
       <c r="E481" t="inlineStr"/>
@@ -12392,7 +12392,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>[1371391.6386005]</t>
+          <t>[1371281.66132225]</t>
         </is>
       </c>
       <c r="E483" t="inlineStr"/>
@@ -12415,7 +12415,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>[3623382.66878689]</t>
+          <t>[3623140.92507672]</t>
         </is>
       </c>
       <c r="E484" t="inlineStr"/>
@@ -12438,7 +12438,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>[38.15883823]</t>
+          <t>[38.1612695]</t>
         </is>
       </c>
       <c r="E485" t="inlineStr"/>
@@ -12461,7 +12461,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>[2.49701458e+09 2.49701458e+09 3.37794715e+07 0.00000000e+00
+          <t>[2.49720247e+09 2.49720247e+09 3.37768590e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12485,7 +12485,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>[2702449.52627567]</t>
+          <t>[2702447.63242067]</t>
         </is>
       </c>
       <c r="E487" t="inlineStr"/>
@@ -12508,7 +12508,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>[7175256.25833561]</t>
+          <t>[7175252.12070514]</t>
         </is>
       </c>
       <c r="E488" t="inlineStr"/>
@@ -12558,7 +12558,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>[0.21999998]</t>
+          <t>[0.22]</t>
         </is>
       </c>
       <c r="E490" t="inlineStr"/>
@@ -12581,7 +12581,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>[0.22140502]</t>
+          <t>[0.22140514]</t>
         </is>
       </c>
       <c r="E491" t="inlineStr"/>
@@ -12604,7 +12604,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>[0.21999998 0.22140502 0.94967181 1.00046036 1.11367713 1.95115072]</t>
+          <t>[0.22       0.22140514 0.94965334 1.00043721 1.11364    1.95101901]</t>
         </is>
       </c>
       <c r="E492" t="inlineStr"/>
@@ -12627,7 +12627,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>[0.22140502 1.11367713 2.12499699]</t>
+          <t>[0.22140514 1.11364    2.12487198]</t>
         </is>
       </c>
       <c r="E493" t="inlineStr"/>
@@ -12650,7 +12650,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>[0.21999998 1.00046036 1.95115072]</t>
+          <t>[0.22       1.00043721 1.95101901]</t>
         </is>
       </c>
       <c r="E494" t="inlineStr"/>
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>[4.28872075 0.         0.        ]</t>
+          <t>[4.28866997 0.         0.        ]</t>
         </is>
       </c>
       <c r="E495" t="inlineStr"/>
@@ -12692,9 +12692,9 @@
       <c r="C496" t="inlineStr"/>
       <c r="D496" t="inlineStr">
         <is>
-          <t>[[ 0.97808852  0.01295424 -0.40849452  0.98464743 -0.56719567]
- [-2.76847845  2.59733002  0.19924016  1.84421263 -0.87230435]
- [-4.7846048   7.96933371  8.3015283  -7.06839007 -3.41786715]]</t>
+          <t>[[ 0.97835845  0.01290938 -0.41179739  0.99055228 -0.57002273]
+ [-2.76930572  2.5963382   0.20891499  1.83127804 -0.8672255 ]
+ [-4.78599653  7.96731545  8.32153312 -7.094456   -3.40839604]]</t>
         </is>
       </c>
       <c r="E496" t="inlineStr"/>
@@ -12713,9 +12713,9 @@
       <c r="C497" t="inlineStr"/>
       <c r="D497" t="inlineStr">
         <is>
-          <t>[[ 0.96961311  0.01649615 -0.40693619  0.97827526 -0.55744832]
- [-2.79943494  2.4124879   0.11334687  1.40023915 -0.12663898]
- [-4.21046578  6.46636514  5.33823026 -2.28155565 -4.31257397]]</t>
+          <t>[[ 0.96988018  0.01644995 -0.41021277  0.98414087 -0.56025823]
+ [-2.80028471  2.41156162  0.12287882  1.38747798 -0.12163371]
+ [-4.21157461  6.46430352  5.35507857 -2.30362777 -4.30417971]]</t>
         </is>
       </c>
       <c r="E497" t="inlineStr"/>
@@ -12734,7 +12734,7 @@
       <c r="C498" t="inlineStr"/>
       <c r="D498" t="inlineStr">
         <is>
-          <t>[[ -1.34289263  12.62720781 -39.80800839  53.45902206 -23.93532885]
+          <t>[[ -1.34259145  12.62045539 -39.78856996  53.43957831 -23.92887228]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -12755,9 +12755,9 @@
       <c r="C499" t="inlineStr"/>
       <c r="D499" t="inlineStr">
         <is>
-          <t>[[ 0.79102467  1.26742065 -3.25757722  3.7905046  -1.5913727 ]
- [-0.55108202  3.16845411 -6.34970613  7.94588308 -3.21354905]
- [ 1.12848279 -0.43154183  7.46214232 -8.79717338  1.6380901 ]]</t>
+          <t>[[ 0.79048042  1.26757541 -3.25486336  3.78663294 -1.58982541]
+ [-0.55069511  3.16621833 -6.34365655  7.93926767 -3.21113434]
+ [ 1.12842649 -0.43268856  7.47004129 -8.80881413  1.64303492]]</t>
         </is>
       </c>
       <c r="E499" t="inlineStr"/>
@@ -12776,9 +12776,9 @@
       <c r="C500" t="inlineStr"/>
       <c r="D500" t="inlineStr">
         <is>
-          <t>[[ 0.77938053  1.28768135 -3.30501822  3.84414594 -1.60618959]
- [-0.66915735  3.45303642 -7.30077981  8.93287785 -3.4159771 ]
- [ 0.71098243  0.33299406  4.30396052 -4.53382443  0.18588742]]</t>
+          <t>[[ 0.77884126  1.28782316 -3.30229696  3.84027822 -1.60464568]
+ [-0.66872446  3.45071857 -7.29482262  8.92657508 -3.41374657]
+ [ 0.71097493  0.33162059  4.31109501 -4.54381959  0.19012907]]</t>
         </is>
       </c>
       <c r="E500" t="inlineStr"/>
@@ -12797,7 +12797,7 @@
       <c r="C501" t="inlineStr"/>
       <c r="D501" t="inlineStr">
         <is>
-          <t>[[ -3.39722424  27.54377885 -75.59445318  90.55332267 -38.10542409]
+          <t>[[ -3.39816701  27.54936054 -75.59354329  90.53686085 -38.0945111 ]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -12822,37 +12822,37 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>[[1.38940715e-04]
- [4.55904847e-04]
- [3.20122231e-04]
- [4.64010151e-03]
- [6.54710227e-03]
- [8.62122784e-03]
- [1.08608381e-02]
- [1.32659726e-02]
- [1.58356894e-02]
- [1.85683207e-02]
- [2.45436839e-02]
- [3.11963980e-02]
- [3.85121112e-02]
- [4.65036610e-02]
- [5.51733019e-02]
- [6.45056665e-02]
- [6.94226311e-02]
- [7.45090088e-02]
- [7.97627600e-02]
- [1.23594799e-01]
- [1.77027459e-01]
- [2.39114695e-01]
- [3.47257397e-01]
- [4.78698179e-01]
- [6.28463570e-01]
- [7.29594990e-01]
- [8.40568469e-01]
- [9.58556986e-01]
- [1.07331412e+00]
- [1.19042916e+00]
- [1.30545175e+00]]</t>
+          <t>[[1.38943829e-04]
+ [4.55905766e-04]
+ [3.20106956e-04]
+ [4.64008306e-03]
+ [6.54707321e-03]
+ [8.62121042e-03]
+ [1.08608544e-02]
+ [1.32661772e-02]
+ [1.58362922e-02]
+ [1.85695295e-02]
+ [2.45464128e-02]
+ [3.12009519e-02]
+ [3.85187887e-02]
+ [4.65125112e-02]
+ [5.51842192e-02]
+ [6.45185475e-02]
+ [6.94363078e-02]
+ [7.45232576e-02]
+ [7.97773597e-02]
+ [1.23609147e-01]
+ [1.77037362e-01]
+ [2.39116374e-01]
+ [3.47249755e-01]
+ [4.78688942e-01]
+ [6.28458831e-01]
+ [7.29594604e-01]
+ [8.40572853e-01]
+ [9.58566383e-01]
+ [1.07332817e+00]
+ [1.19044783e+00]
+ [1.30547505e+00]]</t>
         </is>
       </c>
       <c r="E502" t="inlineStr"/>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>[1.30545175]</t>
+          <t>[1.30547505]</t>
         </is>
       </c>
       <c r="E503" t="inlineStr"/>
@@ -12898,24 +12898,24 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>[[-33863739.80132483]
- [-32458810.78678256]
- [-30740672.69993388]
- [-30202293.31443811]
- [-29662944.25102726]
- [-29121644.09487111]
- [-28583792.7195067 ]
- [-28041943.16216844]
- [-27495002.99396604]
- [-26439293.66241287]
- [-25347955.13371858]
- [-24208338.61119038]
- [-23279136.31635272]
- [-22535633.10125378]
- [-21792129.88615488]
- [-21441583.18977427]
- [-21091036.49339367]
- [-20740489.79701357]]</t>
+          <t>[[-33863690.88866773]
+ [-32458729.79287091]
+ [-30740559.6247678 ]
+ [-30202239.19855307]
+ [-29662949.09442247]
+ [-29121707.89754672]
+ [-28584411.95882652]
+ [-28043117.83813272]
+ [-27496733.10657578]
+ [-26441388.95865573]
+ [-25350415.6135943 ]
+ [-24211164.27469885]
+ [-23281844.63588943]
+ [-22538224.07681884]
+ [-21794603.51774818]
+ [-21443586.0090074 ]
+ [-21092568.50026697]
+ [-20741550.99152588]]</t>
         </is>
       </c>
       <c r="E504" t="inlineStr"/>
@@ -12938,24 +12938,24 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>[[ -3086085.81323177]
- [-10374388.86547915]
- [-13498928.84538622]
- [  2912284.79003139]
- [  2912312.34101361]
- [  2912340.37196493]
- [  2912364.69624453]
- [  2912394.2566323 ]
- [  2912424.82188857]
- [  2912920.36451624]
- [  2913061.43541644]
- [  2913220.56224855]
- [  2913165.78077624]
- [  2912943.11633556]
- [  2913017.02692222]
- [  2912493.31770458]
- [  2912511.13387485]
- [  2912528.73553031]]</t>
+          <t>[[ -3086154.97624959]
+ [-10374472.71212105]
+ [-13498863.57608701]
+ [  2912284.75458243]
+ [  2912312.30620923]
+ [  2912340.33781997]
+ [  2912364.32586176]
+ [  2912393.8931493 ]
+ [  2912424.46592084]
+ [  2912920.27729533]
+ [  2913061.36860698]
+ [  2913220.52258455]
+ [  2913166.24489117]
+ [  2912943.49949671]
+ [  2913017.41021343]
+ [  2912494.09599146]
+ [  2912511.91253024]
+ [  2912529.51454905]]</t>
         </is>
       </c>
       <c r="E505" t="inlineStr"/>
@@ -12978,24 +12978,24 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>[[ -560.1489822 ]
- [-2159.03251905]
- [-4236.0607079 ]
- [-3355.03222407]
- [-3355.0266181 ]
- [-3355.02059256]
- [-3355.01487829]
- [-3355.00787681]
- [-3355.00032166]
- [-3354.90907954]
- [-3354.87016243]
- [-3354.82367746]
- [-3354.8193481 ]
- [-3354.85338357]
- [-3354.82117502]
- [-3354.94384237]
- [-3354.93507694]
- [-3354.92607118]]</t>
+          <t>[[ -560.16401652]
+ [-2159.06126739]
+ [-4236.07156392]
+ [-3355.03222983]
+ [-3355.0266237 ]
+ [-3355.020598  ]
+ [-3355.01494316]
+ [-3355.00794003]
+ [-3355.00038301]
+ [-3354.90908266]
+ [-3354.87015984]
+ [-3354.82366688]
+ [-3354.81922512]
+ [-3354.85328368]
+ [-3354.82107499]
+ [-3354.94363808]
+ [-3354.93487244]
+ [-3354.92586648]]</t>
         </is>
       </c>
       <c r="E506" t="inlineStr"/>
@@ -13018,24 +13018,24 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>[[  -3427.06540599]
- [ -26916.32295169]
- [ -83454.47999688]
- [-102542.73264248]
- [-108125.35191884]
- [-113707.06577714]
- [-119287.867335  ]
- [-124867.71850547]
- [-130446.61160683]
- [-141601.18661971]
- [-152751.43684477]
- [-163897.44514248]
- [-175039.31668966]
- [-186176.46634685]
- [-197308.59348674]
- [-202873.02593154]
- [-208436.11925724]
- [-213997.87565573]]</t>
+          <t>[[  -3427.17392294]
+ [ -26916.78557248]
+ [ -83455.02725174]
+ [-102543.11964437]
+ [-108125.73898123]
+ [-113707.45273495]
+ [-119288.25462457]
+ [-124868.10441073]
+ [-130446.99435319]
+ [-141601.55801817]
+ [-152751.79398229]
+ [-163897.78494795]
+ [-175039.63655569]
+ [-186176.7672896 ]
+ [-197308.87642224]
+ [-202873.30017335]
+ [-208436.3876752 ]
+ [-213998.14118118]]</t>
         </is>
       </c>
       <c r="E507" t="inlineStr"/>
@@ -13058,24 +13058,24 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>[[2.63432389e+07]
- [1.74105677e+08]
- [4.22646099e+08]
- [5.01312414e+08]
- [4.96396477e+08]
- [4.91476750e+08]
- [4.86553414e+08]
- [4.81626668e+08]
- [4.76696746e+08]
- [4.66825893e+08]
- [4.56943413e+08]
- [4.47051387e+08]
- [4.37151335e+08]
- [4.27242918e+08]
- [4.17326020e+08]
- [4.12365557e+08]
- [4.07403203e+08]
- [4.02439103e+08]]</t>
+          <t>[[2.63440057e+07]
+ [1.74108038e+08]
+ [4.22647273e+08]
+ [5.01312368e+08]
+ [4.96396430e+08]
+ [4.91476702e+08]
+ [4.86553361e+08]
+ [4.81626602e+08]
+ [4.76696660e+08]
+ [4.66825754e+08]
+ [4.56943212e+08]
+ [4.47051115e+08]
+ [4.37150987e+08]
+ [4.27242499e+08]
+ [4.17325532e+08]
+ [4.12365040e+08]
+ [4.07402664e+08]
+ [4.02438547e+08]]</t>
         </is>
       </c>
       <c r="E508" t="inlineStr"/>
@@ -13098,24 +13098,24 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>[[ 925641.94365665]
- [2091197.09650497]
- [3798773.38633823]
- [6490314.59902542]
- [6490301.64647439]
- [6490288.67064628]
- [6490286.1492243 ]
- [6490273.01554051]
- [6490259.78427962]
- [6490296.03937005]
- [6490268.35532157]
- [6490239.7372107 ]
- [6490254.54922411]
- [6490228.46730628]
- [6490207.59795461]
- [6490223.72982414]
- [6490213.29514698]
- [6490202.86050342]]</t>
+          <t>[[ 925652.21769021]
+ [2091214.89246739]
+ [3798791.08352944]
+ [6490314.69680958]
+ [6490301.74391663]
+ [6490288.76774339]
+ [6490287.07628086]
+ [6490273.93908096]
+ [6490260.70417696]
+ [6490296.41578718]
+ [6490268.72860595]
+ [6490240.10693338]
+ [6490254.52126754]
+ [6490228.44017368]
+ [6490207.57082312]
+ [6490222.93327906]
+ [6490212.49860472]
+ [6490202.06396379]]</t>
         </is>
       </c>
       <c r="E509" t="inlineStr"/>
@@ -13138,9 +13138,9 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>[[ 2.91228479e+06]
- [-3.35503222e+03]
- [-3.07406727e+07]]</t>
+          <t>[[ 2.91228475e+06]
+ [-3.35503223e+03]
+ [-3.07405596e+07]]</t>
         </is>
       </c>
       <c r="E510" t="inlineStr"/>
@@ -13163,9 +13163,9 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>[[-9.69592261e+04]
- [ 5.06224330e+08]
- [ 6.49031460e+06]]</t>
+          <t>[[-9.69596128e+04]
+ [ 5.06224283e+08]
+ [ 6.49031470e+06]]</t>
         </is>
       </c>
       <c r="E511" t="inlineStr"/>
@@ -13221,8 +13221,8 @@
  10.         10.         10.         10.         10.         10.
  10.         10.         10.         10.         10.         10.
  10.         10.         10.         10.         10.         10.
- 10.          9.99997524  9.99995049  9.99992573  8.66661716  7.3333086
-  6.00000003]</t>
+ 10.         10.         10.         10.          8.66666752  7.33333503
+  6.00000255]</t>
         </is>
       </c>
       <c r="E513" t="inlineStr"/>
@@ -13245,11 +13245,11 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>[0.054943   0.054943   0.054943   0.10225972 0.10225972 0.10225972
- 0.10073409 0.10073409 0.10073409 0.09373654 0.09373654 0.09373654
- 0.08751588 0.08751588 0.08751588 0.08248204 0.08248204 0.08248204
- 0.0675406  0.0675406  0.0675406  0.03725595 0.03725595 0.03725595
- 0.01404628 0.01404628 0.01404628 0.01259864 0.01259864 0.01259864]</t>
+          <t>[0.05494426 0.05494426 0.05494426 0.10224567 0.10224567 0.10224567
+ 0.1006018  0.1006018  0.1006018  0.09369312 0.09369312 0.09369312
+ 0.08752982 0.08752982 0.08752982 0.08259375 0.08259375 0.08259375
+ 0.06757061 0.06757061 0.06757061 0.03724346 0.03724346 0.03724346
+ 0.0140456  0.0140456  0.0140456  0.01259863 0.01259863 0.01259863]</t>
         </is>
       </c>
       <c r="E514" t="inlineStr"/>
@@ -13348,11 +13348,11 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>[1.83676377 1.83676377 1.83676377 3.40231319 3.40231319 3.40231319
- 3.35207007 3.35207007 3.35207007 3.12142181 3.12142181 3.12142181
- 2.91610414 2.91610414 2.91610414 2.74976784 2.74976784 2.74976784
- 2.25504587 2.25504587 2.25504587 1.24769448 1.24769448 1.24769448
- 0.47150259 0.47150142 0.47150025 0.39473397 0.33826786 0.28180174]</t>
+          <t>[1.83680554 1.83680554 1.83680554 3.40185078 3.40185078 3.40185078
+ 3.34771288 3.34771288 3.34771288 3.11998944 3.11998944 3.11998944
+ 2.91656434 2.91656434 2.91656434 2.7534612  2.7534612  2.7534612
+ 2.25604096 2.25604096 2.25604096 1.24727763 1.24727763 1.24727763
+ 0.47148028 0.47148028 0.47148028 0.39473641 0.33826931 0.28180221]</t>
         </is>
       </c>
       <c r="E518" t="inlineStr"/>
@@ -13375,11 +13375,11 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756
- 1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952
+ 1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E519" t="inlineStr"/>
@@ -13402,11 +13402,11 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>[1.04487699 1.04487699 1.04487699 1.93976108 1.93976108 1.93976108
- 1.91097684 1.91097684 1.91097684 1.77889489 1.77889489 1.77889489
- 1.66139573 1.66139573 1.66139573 1.56625757 1.56625757 1.56625756
- 1.28357024 1.28357024 1.28357024 0.70920267 0.70920267 0.70920267
- 0.26772904 0.26772837 0.26772771 0.22413278 0.19209005 0.16004736]</t>
+          <t>[1.04490081 1.04490081 1.04490081 1.93949615 1.93949615 1.93949615
+ 1.90848082 1.90848082 1.90848082 1.77807492 1.77807492 1.77807492
+ 1.66165901 1.66165901 1.66165901 1.56836952 1.56836952 1.56836952
+ 1.28413844 1.28413844 1.28413844 0.70896533 0.70896533 0.70896533
+ 0.26771636 0.26771636 0.26771636 0.22413416 0.19209087 0.16004762]</t>
         </is>
       </c>
       <c r="E520" t="inlineStr"/>
@@ -13429,11 +13429,11 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>[45.41728    45.41728    45.41727999 83.33602078 83.33602079 83.3360208
- 82.13042053 82.13042052 82.13042052 76.58630203 76.58630203 76.58630203
- 71.63774363 71.63774363 71.63774363 67.61951737 67.61951737 67.61951736
- 55.61975444 55.61975442 55.6197544  30.96080759 30.9608076  30.96080762
- 11.75446783 11.75438041 11.75429299  8.5731384   5.39521558  3.11930686]</t>
+          <t>[45.41830148 45.41830148 45.41830148 83.32492866 83.32492866 83.32492866
+ 82.02583302 82.02583302 82.02583302 76.55182254 76.55182254 76.55182254
+ 71.64884942 71.64884942 71.64884942 67.70882823 67.70882823 67.70882823
+ 55.64396406 55.64396406 55.64396406 30.95054111 30.95054111 30.95054111
+ 11.75394248 11.75394248 11.75394248  8.57330591  5.39529059  3.11932561]</t>
         </is>
       </c>
       <c r="E521" t="inlineStr"/>
@@ -13456,11 +13456,11 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868
- 27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411
+ 27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E522" t="inlineStr"/>
@@ -13483,11 +13483,11 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>[22.70864    22.70864    22.70864    41.66801039 41.6680104  41.6680104
- 41.06521026 41.06521026 41.06521026 38.29315101 38.29315101 38.29315102
- 35.81887182 35.81887182 35.81887181 33.80975869 33.80975868 33.80975868
- 27.80987722 27.80987721 27.8098772  15.4804038  15.4804038  15.48040381
-  5.87723392  5.8771902   5.87714649  4.2865692   2.69760779  1.55965343]</t>
+          <t>[22.70915074 22.70915074 22.70915074 41.66246433 41.66246433 41.66246433
+ 41.01291651 41.01291651 41.01291651 38.27591127 38.27591127 38.27591127
+ 35.82442471 35.82442471 35.82442471 33.85441411 33.85441411 33.85441411
+ 27.82198203 27.82198203 27.82198203 15.47527056 15.47527056 15.47527056
+  5.87697124  5.87697124  5.87697124  4.28665295  2.69764529  1.55966281]</t>
         </is>
       </c>
       <c r="E523" t="inlineStr"/>
@@ -13612,36 +13612,36 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>[[-3.38637398e+07]
- [-3.24588108e+07]
- [-3.07406727e+07]
- [-3.02022933e+07]
- [-2.96629443e+07]
- [-2.91216441e+07]
- [-2.85837927e+07]
- [-2.80419432e+07]
- [-2.74950030e+07]
- [-2.64392937e+07]
- [-2.53479551e+07]
- [-2.42083386e+07]
- [-2.32791363e+07]
- [-2.25356331e+07]
- [-2.17921299e+07]
- [-2.14415832e+07]
- [-2.10910365e+07]
- [-2.07404898e+07]
- [-1.76721640e+07]
- [-1.55780768e+07]
- [-1.34825379e+07]
- [-1.18161028e+07]
- [-1.01481843e+07]
- [-8.47880185e+06]
- [-8.09072522e+06]
- [-7.70211664e+06]
- [-7.31314534e+06]
- [-7.00649092e+06]
- [-6.74237634e+06]
- [ 3.75439413e-09]]</t>
+          <t>[[-3.38636909e+07]
+ [-3.24587298e+07]
+ [-3.07405596e+07]
+ [-3.02022392e+07]
+ [-2.96629491e+07]
+ [-2.91217079e+07]
+ [-2.85844120e+07]
+ [-2.80431178e+07]
+ [-2.74967331e+07]
+ [-2.64413890e+07]
+ [-2.53504156e+07]
+ [-2.42111643e+07]
+ [-2.32818446e+07]
+ [-2.25382241e+07]
+ [-2.17946035e+07]
+ [-2.14435860e+07]
+ [-2.10925685e+07]
+ [-2.07415510e+07]
+ [-1.76723062e+07]
+ [-1.55773000e+07]
+ [-1.34808420e+07]
+ [-1.18149567e+07]
+ [-1.01475880e+07]
+ [-8.47875525e+06]
+ [-8.09069629e+06]
+ [-7.70210441e+06]
+ [-7.31314885e+06]
+ [-7.00649251e+06]
+ [-6.74237674e+06]
+ [-2.41561793e-09]]</t>
         </is>
       </c>
       <c r="E527" t="inlineStr"/>
@@ -13664,36 +13664,36 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>[[-3.08608581e+06]
- [-1.03743889e+07]
- [-1.34989288e+07]
- [ 2.91228479e+06]
- [ 2.91231234e+06]
- [ 2.91234037e+06]
- [ 2.91236470e+06]
- [ 2.91239426e+06]
- [ 2.91242482e+06]
- [ 2.91292036e+06]
- [ 2.91306144e+06]
- [ 2.91322056e+06]
- [ 2.91316578e+06]
- [ 2.91294312e+06]
- [ 2.91301703e+06]
- [ 2.91249332e+06]
- [ 2.91251113e+06]
- [ 2.91252874e+06]
- [ 2.91576355e+06]
- [ 2.91661077e+06]
- [ 2.91736537e+06]
- [ 2.91720256e+06]
- [ 2.91833381e+06]
- [ 2.91922658e+06]
- [ 2.91387308e+06]
+          <t>[[-3.08615498e+06]
+ [-1.03744727e+07]
+ [-1.34988636e+07]
+ [ 2.91228475e+06]
+ [ 2.91231231e+06]
+ [ 2.91234034e+06]
+ [ 2.91236433e+06]
+ [ 2.91239389e+06]
+ [ 2.91242447e+06]
+ [ 2.91292028e+06]
+ [ 2.91306137e+06]
+ [ 2.91322052e+06]
+ [ 2.91316624e+06]
+ [ 2.91294350e+06]
+ [ 2.91301741e+06]
+ [ 2.91249410e+06]
+ [ 2.91251191e+06]
+ [ 2.91252951e+06]
+ [ 2.91576520e+06]
+ [ 2.91661242e+06]
+ [ 2.91736702e+06]
+ [ 2.91720038e+06]
+ [ 2.91833164e+06]
+ [ 2.91922441e+06]
+ [ 2.91387307e+06]
  [ 2.91406083e+06]
- [ 2.91419470e+06]
- [ 2.91379896e+06]
- [ 2.91358078e+06]
- [ 1.31558268e+03]]</t>
+ [ 2.91419471e+06]
+ [ 2.91379904e+06]
+ [ 2.91358085e+06]
+ [ 1.31563810e+03]]</t>
         </is>
       </c>
       <c r="E528" t="inlineStr"/>
@@ -13716,36 +13716,36 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>[[ -560.1489822 ]
- [-2159.03251905]
- [-4236.0607079 ]
- [-3355.03222407]
- [-3355.0266181 ]
- [-3355.02059256]
- [-3355.01487829]
- [-3355.00787681]
- [-3355.00032166]
- [-3354.90907954]
- [-3354.87016243]
- [-3354.82367746]
- [-3354.8193481 ]
- [-3354.85338357]
- [-3354.82117502]
- [-3354.94384237]
- [-3354.93507694]
- [-3354.92607118]
- [-3353.90639329]
- [-3353.32416013]
- [-3352.65341641]
- [-3352.06182566]
- [-3350.24068341]
- [-3348.15262212]
- [-3352.7815077 ]
- [-3351.85699315]
- [-3350.87494886]
- [-3350.83621269]
- [-3350.19334229]
- [    4.74684048]]</t>
+          <t>[[ -560.16401652]
+ [-2159.06126739]
+ [-4236.07156392]
+ [-3355.03222983]
+ [-3355.0266237 ]
+ [-3355.020598  ]
+ [-3355.01494316]
+ [-3355.00794003]
+ [-3355.00038301]
+ [-3354.90908266]
+ [-3354.87015984]
+ [-3354.82366688]
+ [-3354.81922512]
+ [-3354.85328368]
+ [-3354.82107499]
+ [-3354.94363808]
+ [-3354.93487244]
+ [-3354.92586648]
+ [-3353.90602718]
+ [-3353.32379186]
+ [-3352.65304542]
+ [-3352.06325097]
+ [-3350.24210199]
+ [-3348.15403191]
+ [-3352.78129943]
+ [-3351.8567796 ]
+ [-3350.87473307]
+ [-3350.83587903]
+ [-3350.19307457]
+ [    4.74704529]]</t>
         </is>
       </c>
       <c r="E529" t="inlineStr"/>
@@ -13768,36 +13768,36 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>[[-3.42706541e+03]
- [-2.69163230e+04]
- [-8.34544800e+04]
- [-1.02542733e+05]
- [-1.08125352e+05]
- [-1.13707066e+05]
- [-1.19287867e+05]
- [-1.24867719e+05]
- [-1.30446612e+05]
- [-1.41601187e+05]
- [-1.52751437e+05]
- [-1.63897445e+05]
- [-1.75039317e+05]
- [-1.86176466e+05]
- [-1.97308593e+05]
- [-2.02873026e+05]
- [-2.08436119e+05]
- [-2.13997876e+05]
- [-2.54231113e+05]
- [-2.94374456e+05]
- [-3.34439945e+05]
- [-3.91457689e+05]
- [-4.48133769e+05]
- [-5.04539806e+05]
- [-5.38214575e+05]
- [-5.71542576e+05]
- [-6.04536130e+05]
- [-6.34984081e+05]
- [-6.64887307e+05]
- [-1.19850988e-04]]</t>
+          <t>[[-3.42717392e+03]
+ [-2.69167856e+04]
+ [-8.34550273e+04]
+ [-1.02543120e+05]
+ [-1.08125739e+05]
+ [-1.13707453e+05]
+ [-1.19288255e+05]
+ [-1.24868104e+05]
+ [-1.30446994e+05]
+ [-1.41601558e+05]
+ [-1.52751794e+05]
+ [-1.63897785e+05]
+ [-1.75039637e+05]
+ [-1.86176767e+05]
+ [-1.97308876e+05]
+ [-2.02873300e+05]
+ [-2.08436388e+05]
+ [-2.13998141e+05]
+ [-2.54231399e+05]
+ [-2.94374820e+05]
+ [-3.34440455e+05]
+ [-3.91458425e+05]
+ [-4.48134577e+05]
+ [-5.04540517e+05]
+ [-5.38215149e+05]
+ [-5.71543004e+05]
+ [-6.04536403e+05]
+ [-6.34984211e+05]
+ [-6.64887311e+05]
+ [-1.19856604e-04]]</t>
         </is>
       </c>
       <c r="E530" t="inlineStr"/>
@@ -13820,36 +13820,36 @@
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>[[ 2.63432389e+07]
- [ 1.74105677e+08]
- [ 4.22646099e+08]
- [ 5.01312414e+08]
- [ 4.96396477e+08]
- [ 4.91476750e+08]
- [ 4.86553414e+08]
- [ 4.81626668e+08]
- [ 4.76696746e+08]
- [ 4.66825893e+08]
- [ 4.56943413e+08]
- [ 4.47051387e+08]
- [ 4.37151335e+08]
- [ 4.27242918e+08]
- [ 4.17326020e+08]
- [ 4.12365557e+08]
- [ 4.07403203e+08]
- [ 4.02439103e+08]
- [ 3.66422437e+08]
- [ 3.30326665e+08]
- [ 2.94207961e+08]
- [ 2.42534673e+08]
- [ 1.90764894e+08]
- [ 1.39028386e+08]
- [ 1.08040213e+08]
- [ 7.70125221e+07]
- [ 4.59739259e+07]
- [ 1.70135072e+07]
- [-1.19282330e+07]
- [ 3.32160984e-02]]</t>
+          <t>[[ 2.63440057e+07]
+ [ 1.74108038e+08]
+ [ 4.22647273e+08]
+ [ 5.01312368e+08]
+ [ 4.96396430e+08]
+ [ 4.91476702e+08]
+ [ 4.86553361e+08]
+ [ 4.81626602e+08]
+ [ 4.76696660e+08]
+ [ 4.66825754e+08]
+ [ 4.56943212e+08]
+ [ 4.47051115e+08]
+ [ 4.37150987e+08]
+ [ 4.27242499e+08]
+ [ 4.17325532e+08]
+ [ 4.12365040e+08]
+ [ 4.07402664e+08]
+ [ 4.02438547e+08]
+ [ 3.66421840e+08]
+ [ 3.30326140e+08]
+ [ 2.94207612e+08]
+ [ 2.42534632e+08]
+ [ 1.90765023e+08]
+ [ 1.39028559e+08]
+ [ 1.08040354e+08]
+ [ 7.70126274e+07]
+ [ 4.59739939e+07]
+ [ 1.70135408e+07]
+ [-1.19282319e+07]
+ [ 3.32183813e-02]]</t>
         </is>
       </c>
       <c r="E531" t="inlineStr"/>
@@ -13872,36 +13872,36 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>[[9.25641944e+05]
- [2.09119710e+06]
- [3.79877339e+06]
- [6.49031460e+06]
- [6.49030165e+06]
- [6.49028867e+06]
- [6.49028615e+06]
- [6.49027302e+06]
- [6.49025978e+06]
- [6.49029604e+06]
- [6.49026836e+06]
- [6.49023974e+06]
- [6.49025455e+06]
- [6.49022847e+06]
- [6.49020760e+06]
- [6.49022373e+06]
- [6.49021330e+06]
- [6.49020286e+06]
- [6.49029228e+06]
- [6.49021650e+06]
- [6.49014049e+06]
- [6.49045954e+06]
- [6.49035022e+06]
- [6.49024079e+06]
- [6.49104706e+06]
- [6.49097967e+06]
- [6.49091220e+06]
- [6.49109162e+06]
- [6.49127060e+06]
- [2.77713178e-09]]</t>
+          <t>[[ 9.25652218e+05]
+ [ 2.09121489e+06]
+ [ 3.79879108e+06]
+ [ 6.49031470e+06]
+ [ 6.49030174e+06]
+ [ 6.49028877e+06]
+ [ 6.49028708e+06]
+ [ 6.49027394e+06]
+ [ 6.49026070e+06]
+ [ 6.49029642e+06]
+ [ 6.49026873e+06]
+ [ 6.49024011e+06]
+ [ 6.49025452e+06]
+ [ 6.49022844e+06]
+ [ 6.49020757e+06]
+ [ 6.49022293e+06]
+ [ 6.49021250e+06]
+ [ 6.49020206e+06]
+ [ 6.49029200e+06]
+ [ 6.49021622e+06]
+ [ 6.49014021e+06]
+ [ 6.49045973e+06]
+ [ 6.49035040e+06]
+ [ 6.49024098e+06]
+ [ 6.49104712e+06]
+ [ 6.49097973e+06]
+ [ 6.49091225e+06]
+ [ 6.49109161e+06]
+ [ 6.49127060e+06]
+ [-2.77714871e-09]]</t>
         </is>
       </c>
       <c r="E532" t="inlineStr"/>
@@ -13924,24 +13924,24 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>[[-12636365.26700381]
- [ 20662938.15956788]
- [ 76322113.16044377]
- [ 51278562.9443131 ]
- [ 50847193.89371801]
- [ 50415943.51961401]
- [ 50714354.46470759]
- [ 50276132.31368244]
- [ 49839042.11543291]
- [ 52483958.34988709]
- [ 51543215.7752804 ]
- [ 50616693.61983293]
- [ 53039535.09287445]
- [ 51911372.44721927]
- [ 50782025.88270485]
- [ 53185624.81629594]
- [ 52579243.49701288]
- [ 51972603.83439305]]</t>
+          <t>[[-12635880.9640691 ]
+ [ 20663041.98180812]
+ [ 76320720.74468386]
+ [ 51285374.51228298]
+ [ 50853931.12645442]
+ [ 50422606.34205623]
+ [ 50778600.7906476 ]
+ [ 50339656.66502669]
+ [ 49901845.09443352]
+ [ 52506834.25059135]
+ [ 51565545.82607796]
+ [ 50638483.10137754]
+ [ 53030358.91809265]
+ [ 51902400.66891311]
+ [ 50773259.12650026]
+ [ 53114840.88269465]
+ [ 52509424.23210759]
+ [ 51903750.61315396]]</t>
         </is>
       </c>
       <c r="E533" t="inlineStr"/>
@@ -13964,24 +13964,24 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>[[ 3055444.05324575]
- [10159034.27079205]
- [13337364.62744953]
- [ 1890769.9432749 ]
- [ 1890783.36935514]
- [ 1890797.04147561]
- [ 1919140.56366769]
- [ 1919155.23284717]
- [ 1919170.42192583]
- [ 2061214.17619018]
- [ 2061291.67126007]
- [ 2061379.25542096]
- [ 2206437.2838629 ]
- [ 2206301.4410924 ]
- [ 2206344.47153587]
- [ 2339432.67221464]
- [ 2339443.27570075]
- [ 2339453.74222913]]</t>
+          <t>[[ 3055441.74440007]
+ [10158884.92429425]
+ [13337000.15539991]
+ [ 1891026.8515836 ]
+ [ 1891040.27987781]
+ [ 1891053.95425333]
+ [ 1921637.4277067 ]
+ [ 1921652.11947396]
+ [ 1921667.3321353 ]
+ [ 2062160.13592804]
+ [ 2062237.67805523]
+ [ 2062325.31768594]
+ [ 2206089.51959502]
+ [ 2205953.6496422 ]
+ [ 2205996.6733023 ]
+ [ 2336296.06531617]
+ [ 2336306.65465786]
+ [ 2336317.10722298]]</t>
         </is>
       </c>
       <c r="E534" t="inlineStr"/>
@@ -14006,17 +14006,17 @@
         <is>
           <t>[[       -0.        ]
  [       -0.        ]
- [ -9732465.99882087]
- [-10004702.85451061]
- [ -9200143.16080469]
- [ -8401829.29263714]
- [ -7726340.76396954]
- [ -6928979.73885455]
- [ -6138592.39229669]
- [ -5344706.86299601]
- [ -3695869.84909273]
- [ -2087533.34225309]
- [  -693589.93844489]
+ [ -9732242.20718175]
+ [-10006091.16323108]
+ [ -9201419.82404184]
+ [ -8402995.17714271]
+ [ -7736603.67782491]
+ [ -6938183.51654293]
+ [ -6146746.29695238]
+ [ -5347207.46874079]
+ [ -3697599.02029112]
+ [ -2088510.02774211]
+ [  -693478.54798428]
  [       -0.        ]
  [       -0.        ]
  [       -0.        ]
@@ -14080,24 +14080,24 @@
       <c r="C537" t="inlineStr"/>
       <c r="D537" t="inlineStr">
         <is>
-          <t>[[0.06969037]
- [0.13805956]
- [0.43152998]
- [0.29014998]
- [0.28544156]
- [0.28078293]
- [0.28022287]
- [0.27559439]
- [0.27102566]
- [0.28214909]
- [0.27269154]
- [0.26358189]
- [0.27228602]
- [0.26478544]
- [0.25905638]
- [0.27133702]
- [0.2682614 ]
- [0.26518469]]</t>
+          <t>[[0.06968809]
+ [0.13805911]
+ [0.43152168]
+ [0.29018871]
+ [0.28547957]
+ [0.28082021]
+ [0.28057935]
+ [0.27594399]
+ [0.27136846]
+ [0.28227259]
+ [0.27281007]
+ [0.2636956 ]
+ [0.27223896]
+ [0.2647397 ]
+ [0.25901168]
+ [0.27097588]
+ [0.26790516]
+ [0.26483335]]</t>
         </is>
       </c>
       <c r="E537" t="inlineStr"/>
@@ -14116,24 +14116,24 @@
       <c r="C538" t="inlineStr"/>
       <c r="D538" t="inlineStr">
         <is>
-          <t>[[0.11037065]
- [0.160393  ]
- [0.36934015]
- [0.03903354]
- [0.03734319]
- [0.03575344]
- [0.03503673]
- [0.03365031]
- [0.03239582]
- [0.04286295]
- [0.0387845 ]
- [0.03552116]
- [0.03697611]
- [0.03565401]
- [0.03469926]
- [0.03448469]
- [0.03401592]
- [0.03354825]]</t>
+          <t>[[0.11036654]
+ [0.16038735]
+ [0.36932012]
+ [0.03904128]
+ [0.03735064]
+ [0.03576062]
+ [0.03510452]
+ [0.03371574]
+ [0.03245907]
+ [0.04290113]
+ [0.03881778]
+ [0.03555013]
+ [0.03697096]
+ [0.03564942]
+ [0.03469472]
+ [0.03442359]
+ [0.03395507]
+ [0.03348766]]</t>
         </is>
       </c>
       <c r="E538" t="inlineStr"/>
@@ -14152,24 +14152,24 @@
       <c r="C539" t="inlineStr"/>
       <c r="D539" t="inlineStr">
         <is>
-          <t>[[0.11710657]
- [0.25874216]
- [0.49844803]
- [0.31086382]
- [0.30743227]
- [0.3039964 ]
- [0.30501945]
- [0.30152872]
- [0.29802916]
- [0.31235692]
- [0.30483632]
- [0.29723401]
- [0.31018159]
- [0.30273593]
- [0.29528735]
- [0.3090728 ]
- [0.30516217]
- [0.30125101]]</t>
+          <t>[[0.11710529]
+ [0.25874009]
+ [0.49844087]
+ [0.31090762]
+ [0.30747567]
+ [0.3040394 ]
+ [0.30541513]
+ [0.30192067]
+ [0.29841737]
+ [0.31250439]
+ [0.30498084]
+ [0.29737554]
+ [0.31013975]
+ [0.30269496]
+ [0.29524725]
+ [0.30866728]
+ [0.30476097]
+ [0.30085413]]</t>
         </is>
       </c>
       <c r="E539" t="inlineStr"/>
@@ -14192,36 +14192,36 @@
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>[[-1.26363653e+07]
- [ 2.06629382e+07]
- [ 7.63221132e+07]
- [ 5.12785629e+07]
- [ 5.08471939e+07]
- [ 5.04159435e+07]
- [ 5.07143545e+07]
- [ 5.02761323e+07]
- [ 4.98390421e+07]
- [ 5.24839583e+07]
- [ 5.15432158e+07]
- [ 5.06166936e+07]
- [ 5.30395351e+07]
- [ 5.19113724e+07]
- [ 5.07820259e+07]
- [ 5.31856248e+07]
- [ 5.25792435e+07]
- [ 5.19726038e+07]
- [ 5.80432046e+07]
- [ 5.24820957e+07]
- [ 4.69175105e+07]
- [ 6.88657817e+07]
- [ 5.34815815e+07]
- [ 3.81093584e+07]
- [ 7.47557445e+07]
- [ 4.91844089e+07]
- [ 2.36052203e+07]
- [ 7.84991043e+05]
- [-2.21756242e+06]
- [ 7.09906842e-02]]</t>
+          <t>[[-1.26358810e+07]
+ [ 2.06630420e+07]
+ [ 7.63207207e+07]
+ [ 5.12853745e+07]
+ [ 5.08539311e+07]
+ [ 5.04226063e+07]
+ [ 5.07786008e+07]
+ [ 5.03396567e+07]
+ [ 4.99018451e+07]
+ [ 5.25068343e+07]
+ [ 5.15655458e+07]
+ [ 5.06384831e+07]
+ [ 5.30303589e+07]
+ [ 5.19024007e+07]
+ [ 5.07732591e+07]
+ [ 5.31148409e+07]
+ [ 5.25094242e+07]
+ [ 5.19037506e+07]
+ [ 5.80178279e+07]
+ [ 5.24595530e+07]
+ [ 4.68978223e+07]
+ [ 6.88895071e+07]
+ [ 5.34998212e+07]
+ [ 3.81220758e+07]
+ [ 7.47593356e+07]
+ [ 4.91864764e+07]
+ [ 2.36060224e+07]
+ [ 7.84894645e+05]
+ [-2.21764101e+06]
+ [ 7.09952690e-02]]</t>
         </is>
       </c>
       <c r="E540" t="inlineStr"/>
@@ -14244,36 +14244,36 @@
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>[[3.05544405e+06]
- [1.01590343e+07]
- [1.33373646e+07]
- [1.89076994e+06]
- [1.89078337e+06]
- [1.89079704e+06]
- [1.91914056e+06]
- [1.91915523e+06]
- [1.91917042e+06]
- [2.06121418e+06]
- [2.06129167e+06]
- [2.06137926e+06]
- [2.20643728e+06]
- [2.20630144e+06]
- [2.20634447e+06]
- [2.33943267e+06]
- [2.33944328e+06]
- [2.33945374e+06]
- [2.85505778e+06]
- [2.85571101e+06]
- [2.85629207e+06]
- [5.16153149e+06]
- [5.16310893e+06]
- [5.16435009e+06]
- [1.36447663e+07]
- [1.36454796e+07]
- [1.36459916e+07]
- [1.65336440e+07]
- [1.99803866e+07]
- [8.22001229e+03]]</t>
+          <t>[[3.05544174e+06]
+ [1.01588849e+07]
+ [1.33370002e+07]
+ [1.89102685e+06]
+ [1.89104028e+06]
+ [1.89105395e+06]
+ [1.92163743e+06]
+ [1.92165212e+06]
+ [1.92166733e+06]
+ [2.06216014e+06]
+ [2.06223768e+06]
+ [2.06232532e+06]
+ [2.20608952e+06]
+ [2.20595365e+06]
+ [2.20599667e+06]
+ [2.33629607e+06]
+ [2.33630665e+06]
+ [2.33631711e+06]
+ [2.85380007e+06]
+ [2.85445301e+06]
+ [2.85503382e+06]
+ [5.16325317e+06]
+ [5.16483115e+06]
+ [5.16607273e+06]
+ [1.36454084e+07]
+ [1.36460811e+07]
+ [1.36465524e+07]
+ [1.65335188e+07]
+ [1.99802782e+07]
+ [8.22034497e+03]]</t>
         </is>
       </c>
       <c r="E541" t="inlineStr"/>
@@ -14298,34 +14298,34 @@
         <is>
           <t>[[-0.00000000e+00]
  [-0.00000000e+00]
- [-9.73246600e+06]
- [-1.00047029e+07]
- [-9.20014316e+06]
- [-8.40182929e+06]
- [-7.72634076e+06]
- [-6.92897974e+06]
- [-6.13859239e+06]
- [-5.34470686e+06]
- [-3.69586985e+06]
- [-2.08753334e+06]
- [-6.93589938e+05]
+ [-9.73224221e+06]
+ [-1.00060912e+07]
+ [-9.20141982e+06]
+ [-8.40299518e+06]
+ [-7.73660368e+06]
+ [-6.93818352e+06]
+ [-6.14674630e+06]
+ [-5.34720747e+06]
+ [-3.69759902e+06]
+ [-2.08851003e+06]
+ [-6.93478548e+05]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
- [-3.98502792e+03]
- [-1.04898421e+04]
- [-1.17514625e+04]
- [-1.26799713e+04]
- [-2.46592922e+04]
- [-2.62245650e+04]
- [-2.75371116e+04]
- [-7.56888192e+04]
- [-7.73698018e+04]
- [-7.89422695e+04]
- [-8.36407781e+04]
- [-7.28434014e+04]
- [-6.16092799e+04]]</t>
+ [-3.97959293e+03]
+ [-1.04851519e+04]
+ [-1.17462082e+04]
+ [-1.26743019e+04]
+ [-2.46675954e+04]
+ [-2.62333952e+04]
+ [-2.75463837e+04]
+ [-7.56925981e+04]
+ [-7.73738565e+04]
+ [-7.89466023e+04]
+ [-8.36413809e+04]
+ [-7.28437895e+04]
+ [-6.16094460e+04]]</t>
         </is>
       </c>
       <c r="E542" t="inlineStr"/>
@@ -14396,36 +14396,36 @@
       <c r="C544" t="inlineStr"/>
       <c r="D544" t="inlineStr">
         <is>
-          <t>[[6.96903653e-02]
- [1.38059564e-01]
- [4.31529976e-01]
- [2.90149981e-01]
- [2.85441565e-01]
- [2.80782932e-01]
- [2.80222875e-01]
- [2.75594385e-01]
- [2.71025656e-01]
- [2.82149086e-01]
- [2.72691538e-01]
- [2.63581886e-01]
- [2.72286025e-01]
- [2.64785439e-01]
- [2.59056377e-01]
- [2.71337017e-01]
- [2.68261405e-01]
- [2.65194797e-01]
- [2.96359496e-01]
- [2.68186958e-01]
- [2.40022591e-01]
- [3.53319028e-01]
- [2.75901434e-01]
- [1.99197379e-01]
- [3.99014079e-01]
- [2.77764353e-01]
- [1.70068404e-01]
- [1.45736911e-01]
- [1.76394125e-01]
- [3.21663572e-04]]</t>
+          <t>[[6.96880851e-02]
+ [1.38059113e-01]
+ [4.31521680e-01]
+ [2.90188714e-01]
+ [2.85479570e-01]
+ [2.80820215e-01]
+ [2.80579355e-01]
+ [2.75943992e-01]
+ [2.71368464e-01]
+ [2.82272587e-01]
+ [2.72810065e-01]
+ [2.63695598e-01]
+ [2.72238961e-01]
+ [2.64739698e-01]
+ [2.59011677e-01]
+ [2.70975884e-01]
+ [2.67905164e-01]
+ [2.64843442e-01]
+ [2.96229920e-01]
+ [2.68071737e-01]
+ [2.39921814e-01]
+ [3.53440688e-01]
+ [2.75995473e-01]
+ [1.99263851e-01]
+ [3.99033212e-01]
+ [2.77776138e-01]
+ [1.70074791e-01]
+ [1.45735795e-01]
+ [1.76393197e-01]
+ [3.21665056e-04]]</t>
         </is>
       </c>
       <c r="E544" t="inlineStr"/>
@@ -14444,36 +14444,36 @@
       <c r="C545" t="inlineStr"/>
       <c r="D545" t="inlineStr">
         <is>
-          <t>[[0.11037065]
- [0.160393  ]
- [0.36934015]
- [0.03903354]
- [0.03734319]
- [0.03575344]
- [0.03503673]
- [0.03365031]
- [0.03239582]
- [0.04286295]
- [0.0387845 ]
- [0.03552116]
- [0.03697611]
- [0.03565401]
- [0.03469926]
- [0.03448469]
- [0.03401592]
- [0.0335454 ]
- [0.05131757]
- [0.04764311]
- [0.04404006]
- [0.13161496]
- [0.12411908]
- [0.11675638]
- [0.81219807]
- [0.79839329]
- [0.78455941]
- [0.97839034]
- [1.00000001]
- [0.01044303]]</t>
+          <t>[[0.11036654]
+ [0.16038735]
+ [0.36932012]
+ [0.03904128]
+ [0.03735064]
+ [0.03576062]
+ [0.03510452]
+ [0.03371574]
+ [0.03245907]
+ [0.04290113]
+ [0.03881778]
+ [0.03555013]
+ [0.03697096]
+ [0.03564942]
+ [0.03469472]
+ [0.03442359]
+ [0.03395507]
+ [0.0334848 ]
+ [0.05127827]
+ [0.04760464]
+ [0.04400249]
+ [0.13169865]
+ [0.1242007 ]
+ [0.11683583]
+ [0.81228613]
+ [0.79848008]
+ [0.78464488]
+ [0.97839037]
+ [1.        ]
+ [0.01044309]]</t>
         </is>
       </c>
       <c r="E545" t="inlineStr"/>
@@ -14492,36 +14492,36 @@
       <c r="C546" t="inlineStr"/>
       <c r="D546" t="inlineStr">
         <is>
-          <t>[[2.93071281e-01]
- [5.57207991e-01]
- [1.00002103e+00]
- [5.87511907e-01]
- [5.80173898e-01]
- [5.72836663e-01]
- [5.74345676e-01]
- [5.66903997e-01]
- [5.59447941e-01]
- [5.86641873e-01]
- [5.70589093e-01]
- [5.54330313e-01]
- [5.78708854e-01]
- [5.63615354e-01]
- [5.48563123e-01]
- [5.75171233e-01]
- [5.67302290e-01]
- [5.59444648e-01]
- [6.13637673e-01]
- [5.47540121e-01]
- [4.82231392e-01]
- [7.39844465e-01]
- [5.85515266e-01]
- [4.34298898e-01]
- [9.98155686e-01]
- [7.61582209e-01]
- [5.28263172e-01]
- [4.21725246e-01]
- [5.65791580e-01]
- [5.15420000e-10]]</t>
+          <t>[[2.93066037e-01]
+ [5.57199581e-01]
+ [1.00000035e+00]
+ [5.87597019e-01]
+ [5.80258158e-01]
+ [5.72920070e-01]
+ [5.75128859e-01]
+ [5.67679076e-01]
+ [5.60214891e-01]
+ [5.86936077e-01]
+ [5.70876810e-01]
+ [5.54611422e-01]
+ [5.78631721e-01]
+ [5.63539937e-01]
+ [5.48489420e-01]
+ [5.74383505e-01]
+ [5.66523192e-01]
+ [5.58674171e-01]
+ [6.13358020e-01]
+ [5.47285381e-01]
+ [4.82001324e-01]
+ [7.40092412e-01]
+ [5.85714897e-01]
+ [4.34451067e-01]
+ [9.98210222e-01]
+ [7.61619028e-01]
+ [5.28285310e-01]
+ [4.21719023e-01]
+ [5.65784510e-01]
+ [5.15455910e-10]]</t>
         </is>
       </c>
       <c r="E546" t="inlineStr"/>
@@ -14652,9 +14652,9 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>[ 927.99815936 1070.12742471 1170.96499623 1251.15492773 1344.7463733
- 1422.65663252 1490.05546077 1526.70536514 1561.05280271 1593.42204527
- 1387.33212347 1189.05587167  992.78219031]</t>
+          <t>[ 927.99815941 1070.12742489 1170.96499657 1251.15492825 1344.74637368
+ 1422.65663272 1490.05546077 1526.70959182 1561.06149956 1593.43543743
+ 1387.3406018  1189.06011169  992.78259162]</t>
         </is>
       </c>
       <c r="E551" t="inlineStr"/>
@@ -14773,9 +14773,9 @@
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>[ 927.99815936 1070.12742471 1170.96499623 1251.15492773 1344.7463733
- 1422.65663252 1490.05546077 1526.70536514 1561.05280271 1593.42204527
- 1387.33212347 1189.05587167  992.78219031]</t>
+          <t>[ 927.99815941 1070.12742489 1170.96499657 1251.15492825 1344.74637368
+ 1422.65663272 1490.05546077 1526.70959182 1561.06149956 1593.43543743
+ 1387.3406018  1189.06011169  992.78259162]</t>
         </is>
       </c>
       <c r="E556" t="inlineStr"/>
@@ -14963,10 +14963,10 @@
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>[ -927.99815936 -1070.12742471 -1170.96499623 -1251.15492773
- -1344.7463733  -1422.65663252 -1490.05546077 -1526.70536514
- -1561.05280271 -1593.42204527 -1387.33212347 -1189.05587167
-  -992.78219031]</t>
+          <t>[ -927.99815941 -1070.12742489 -1170.96499657 -1251.15492825
+ -1344.74637368 -1422.65663272 -1490.05546077 -1526.70959182
+ -1561.06149956 -1593.43543743 -1387.3406018  -1189.06011169
+  -992.78259162]</t>
         </is>
       </c>
       <c r="E564" t="inlineStr"/>
@@ -15010,7 +15010,7 @@
       <c r="C566" t="inlineStr"/>
       <c r="D566" t="inlineStr">
         <is>
-          <t>[148.05908738 268.41350967 711.92946113 634.98633319]</t>
+          <t>[147.99333454 268.50355199 711.96671841 634.9897109 ]</t>
         </is>
       </c>
       <c r="E566" t="inlineStr"/>
@@ -15029,7 +15029,7 @@
       <c r="C567" t="inlineStr"/>
       <c r="D567" t="inlineStr">
         <is>
-          <t>[1.         1.         0.99999257 0.60000446]</t>
+          <t>[1.         1.         1.         0.60000026]</t>
         </is>
       </c>
       <c r="E567" t="inlineStr"/>
@@ -15048,7 +15048,7 @@
       <c r="C568" t="inlineStr"/>
       <c r="D568" t="inlineStr">
         <is>
-          <t>[1.         1.         0.99999257 0.60000446]</t>
+          <t>[1.         1.         1.         0.60000026]</t>
         </is>
       </c>
       <c r="E568" t="inlineStr"/>
@@ -15067,7 +15067,7 @@
       <c r="C569" t="inlineStr"/>
       <c r="D569" t="inlineStr">
         <is>
-          <t>[0.55160818 0.37702122 0.89693748]</t>
+          <t>[0.55117831 0.37712936 0.89698062]</t>
         </is>
       </c>
       <c r="E569" t="inlineStr"/>
@@ -15111,8 +15111,8 @@
       <c r="D571" t="inlineStr">
         <is>
           <t>[5.         5.         5.         5.         5.         5.
- 5.         4.99998762 4.99997524 4.99996287 4.33330858 3.6666543
- 3.00000001]</t>
+ 5.         5.         5.         5.         4.33333376 3.66666752
+ 3.00000128]</t>
         </is>
       </c>
       <c r="E571" t="inlineStr"/>
@@ -15364,8 +15364,8 @@
       <c r="D582" t="inlineStr">
         <is>
           <t>[10.         10.         10.         10.         10.         10.
- 10.          9.99997524  9.99995049  9.99992573  8.66661716  7.3333086
-  6.00000003]</t>
+ 10.         10.         10.         10.          8.66666752  7.33333503
+  6.00000255]</t>
         </is>
       </c>
       <c r="E582" t="inlineStr"/>
@@ -15618,7 +15618,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>[17589.35779277  9732.01691963  3677.71108563  2638.48929575]</t>
+          <t>[17597.11951627  9728.7655043   3677.54621408  2638.5006093 ]</t>
         </is>
       </c>
       <c r="E593" t="inlineStr">
@@ -15645,7 +15645,7 @@
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>[216917.0422353  120747.14965849  45842.08359787  21041.34075188]</t>
+          <t>[217011.4598477  120707.11032995  45840.37568999  21041.63330096]</t>
         </is>
       </c>
       <c r="E594" t="inlineStr">
@@ -15672,7 +15672,7 @@
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>[216917.0422353  120747.14965849  45842.08359787  21041.34075188]</t>
+          <t>[217011.4598477  120707.11032995  45840.37568999  21041.63330096]</t>
         </is>
       </c>
       <c r="E595" t="inlineStr">
@@ -15699,7 +15699,7 @@
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>[5.19810789e+12 2.89353342e+12 1.09854023e+12 5.04225755e+11]</t>
+          <t>[5.20037047e+12 2.89257394e+12 1.09849930e+12 5.04232765e+11]</t>
         </is>
       </c>
       <c r="E596" t="inlineStr">
@@ -15726,7 +15726,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>[5.19810789e+12 2.89353342e+12 1.09854023e+12 5.04225755e+11]</t>
+          <t>[5.20037047e+12 2.89257394e+12 1.09849930e+12 5.04232765e+11]</t>
         </is>
       </c>
       <c r="E597" t="inlineStr">
@@ -15753,7 +15753,7 @@
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>[4.12209956e+12 2.29457200e+12 8.71142399e+11 3.99851024e+11]</t>
+          <t>[4.12389379e+12 2.29381113e+12 8.71109943e+11 3.99856583e+11]</t>
         </is>
       </c>
       <c r="E598" t="inlineStr">
@@ -15780,7 +15780,7 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>[4.21503901e+11 2.33213921e+11 8.81311068e+10 6.32276371e+10]</t>
+          <t>[4.21689900e+11 2.33136005e+11 8.81271559e+10 6.32279082e+10]</t>
         </is>
       </c>
       <c r="E599" t="inlineStr">
@@ -15888,10 +15888,10 @@
       </c>
       <c r="D603" t="inlineStr">
         <is>
-          <t>[[0.         0.         0.47449146 0.19237769 0.19237769 0.        ]
- [0.         0.         0.85758174 0.34559822 0.34559822 0.        ]
- [0.         0.         2.26934629 0.91029556 0.91029556 0.        ]
- [0.         0.         3.16317372 1.58658355 1.58658355 0.        ]]</t>
+          <t>[[0.         0.         0.47428217 0.19229399 0.19229399 0.        ]
+ [0.         0.         0.85786835 0.34571286 0.34571286 0.        ]
+ [0.         0.         2.26944803 0.91033285 0.91033285 0.        ]
+ [0.         0.         3.16316016 1.58656911 1.58656911 0.        ]]</t>
         </is>
       </c>
       <c r="E603" t="inlineStr"/>
@@ -15914,10 +15914,10 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>[[0.77907696 0.77907696 0.         0.         0.         0.09618885]
- [1.41003417 1.41003417 0.         0.         0.         0.17279911]
- [3.73512895 3.73512895 0.         0.         0.         0.45514778]
- [5.20589182 5.20589182 0.         0.         0.         0.79329177]]</t>
+          <t>[[0.77873224 0.77873224 0.         0.         0.         0.096147  ]
+ [1.41050621 1.41050621 0.         0.         0.         0.17285643]
+ [3.73529653 3.73529653 0.         0.         0.         0.45516643]
+ [5.20586951 5.20586951 0.         0.         0.         0.79328455]]</t>
         </is>
       </c>
       <c r="E604" t="inlineStr"/>
@@ -15940,7 +15940,7 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>[611.05890541]</t>
+          <t>[611.07198298]</t>
         </is>
       </c>
       <c r="E605" t="inlineStr"/>
@@ -15963,7 +15963,7 @@
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>[3551873.58954871]</t>
+          <t>[3552111.19562842]</t>
         </is>
       </c>
       <c r="E606" t="inlineStr"/>
@@ -15987,7 +15987,7 @@
       <c r="D607" t="inlineStr">
         <is>
           <t>[10.         10.         10.         10.         10.         10.
-  9.99998762  9.99996287  9.99993811  9.33327145  7.99996288  6.66665431]</t>
+ 10.         10.         10.          9.33333376  8.00000128  6.66666879]</t>
         </is>
       </c>
       <c r="E607" t="inlineStr"/>
@@ -16010,8 +16010,8 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>[0.07226844 0.07226844 0.07226844 0.03986387 0.03986387 0.03986387
- 0.01502952 0.01502952 0.01502952 0.01348054 0.01348054 0.01348054]</t>
+          <t>[0.07230055 0.07230055 0.07230055 0.0398505  0.0398505  0.0398505
+ 0.01502879 0.01502879 0.01502879 0.01348054 0.01348054 0.01348054]</t>
         </is>
       </c>
       <c r="E608" t="inlineStr"/>
@@ -16058,18 +16058,18 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>[[62560592.24955206]
- [57118913.21692217]
- [51657623.37910295]
- [77603104.49921101]
- [62403597.63490295]
- [47181321.22788477]
- [98833654.66306756]
- [73418776.93190178]
- [47971001.05208147]
- [32082309.88272005]
- [ 5154061.50257463]
- [ 2443377.97383584]]</t>
+          <t>[[62533247.86468507]
+ [57094360.02756426]
+ [51635882.6324526 ]
+ [77629734.73374239]
+ [62424797.12420073]
+ [47197046.31214205]
+ [98838353.75393046]
+ [73421844.79844429]
+ [47972692.84023707]
+ [32081832.35823008]
+ [ 5153955.83139599]
+ [ 2443318.09259828]]</t>
         </is>
       </c>
       <c r="E610" t="inlineStr"/>
@@ -16092,18 +16092,18 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>[[ 2852498.19882127]
- [ 2853185.41420811]
- [ 2853810.46137895]
- [ 5158081.90834785]
- [ 5159835.26624356]
- [ 5161254.77893212]
- [13643010.39695831]
- [13643899.63615655]
- [13644592.56066975]
- [16532506.41285849]
- [19979485.30142684]
- [25139131.83263069]]</t>
+          <t>[[ 2851240.3400633 ]
+ [ 2851927.25201427]
+ [ 2852552.02298979]
+ [ 5159803.31014614]
+ [ 5161557.25898389]
+ [ 5162977.25199336]
+ [13643652.41933427]
+ [13644501.04750292]
+ [13645153.34728844]
+ [16532381.19036978]
+ [19979376.81085296]
+ [25139075.36049255]]</t>
         </is>
       </c>
       <c r="E611" t="inlineStr"/>
@@ -16126,18 +16126,18 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>[[-10489.84214684]
- [-11751.46253675]
- [-12679.97133248]
- [-24659.29224808]
- [-26224.56495359]
- [-27537.11155953]
- [-75688.81917952]
- [-77369.80177958]
- [-78942.26949921]
- [-83640.77814934]
- [-72843.40143935]
- [-61609.27985903]]</t>
+          <t>[[-10485.1519431 ]
+ [-11746.20824039]
+ [-12674.30188412]
+ [-24667.59542182]
+ [-26233.39517596]
+ [-27546.3837333 ]
+ [-75692.59810949]
+ [-77373.85645509]
+ [-78946.60230046]
+ [-83641.38085352]
+ [-72843.78952856]
+ [-61609.44601345]]</t>
         </is>
       </c>
       <c r="E612" t="inlineStr"/>
@@ -16190,18 +16190,18 @@
       <c r="C614" t="inlineStr"/>
       <c r="D614" t="inlineStr">
         <is>
-          <t>[[0.3192605 ]
- [0.29167668]
- [0.26401245]
- [0.39743338]
- [0.32074937]
- [0.24434833]
- [0.51712041]
- [0.39253612]
- [0.27221325]
- [0.21891275]
- [0.17800602]
- [0.22185501]]</t>
+          <t>[[0.31912095]
+ [0.29155128]
+ [0.26390129]
+ [0.39756972]
+ [0.32085829]
+ [0.24442977]
+ [0.51714499]
+ [0.39255261]
+ [0.27222316]
+ [0.2189102 ]
+ [0.17800499]
+ [0.2218545 ]]</t>
         </is>
       </c>
       <c r="E614" t="inlineStr"/>
@@ -16220,18 +16220,18 @@
       <c r="C615" t="inlineStr"/>
       <c r="D615" t="inlineStr">
         <is>
-          <t>[[0.05130589]
- [0.04762852]
- [0.04402332]
- [0.13156119]
- [0.12406072]
- [0.11669484]
- [0.81198969]
- [0.79817827]
- [0.78433878]
- [0.97817161]
- [0.99988672]
- [1.04459152]]</t>
+          <t>[[0.0512666 ]
+ [0.04759005]
+ [0.04398575]
+ [0.13164485]
+ [0.12414232]
+ [0.11677426]
+ [0.81207772]
+ [0.79826504]
+ [0.78442421]
+ [0.97817163]
+ [0.99988671]
+ [1.04459199]]</t>
         </is>
       </c>
       <c r="E615" t="inlineStr"/>
@@ -16250,18 +16250,18 @@
       <c r="C616" t="inlineStr"/>
       <c r="D616" t="inlineStr">
         <is>
-          <t>[[0.91447053]
- [0.8260914 ]
- [0.73802771]
- [1.13366963]
- [0.92021312]
- [0.70851687]
- [1.6117519 ]
- [1.28439063]
- [0.95872759]
- [0.86174713]
- [0.6494268 ]
- [0.83178297]]</t>
+          <t>[[0.91405794]
+ [0.82571348]
+ [0.73768446]
+ [1.13403784]
+ [0.92051604]
+ [0.7087547 ]
+ [1.61182393]
+ [1.28444081]
+ [0.95875999]
+ [0.86173195]
+ [0.64941837]
+ [0.83177631]]</t>
         </is>
       </c>
       <c r="E616" t="inlineStr"/>
@@ -16377,7 +16377,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>[0.26360487]</t>
+          <t>[0.26360761]</t>
         </is>
       </c>
       <c r="E621" t="inlineStr"/>
@@ -16400,7 +16400,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>[0.26685509]</t>
+          <t>[0.26685824]</t>
         </is>
       </c>
       <c r="E622" t="inlineStr"/>
@@ -16423,7 +16423,7 @@
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>[0.26360487 0.26685509 0.84852533 1.0237949  1.21826429 2.6636403 ]</t>
+          <t>[0.26360761 0.26685824 0.84851366 1.02383396 1.21832108 2.66402667]</t>
         </is>
       </c>
       <c r="E623" t="inlineStr"/>
@@ -16442,9 +16442,9 @@
       <c r="C624" t="inlineStr"/>
       <c r="D624" t="inlineStr">
         <is>
-          <t>[[   0.85272565    0.44395627   -1.26031726    1.72313488   -0.75949955]
- [  29.99542099   27.6429546  -142.04567276  169.50940094  -84.10210377]
- [ -63.59858633  155.08415172 -267.07243935  337.20916307 -160.6222891 ]]</t>
+          <t>[[   0.85219128    0.4441617    -1.25783185    1.71953079   -0.75805193]
+ [  29.95590225   27.70099055 -142.06194903  169.48065356  -84.07559734]
+ [ -63.59642846  155.01895308 -266.93924982  337.12711001 -160.61038481]]</t>
         </is>
       </c>
       <c r="E624" t="inlineStr"/>
@@ -16463,9 +16463,9 @@
       <c r="C625" t="inlineStr"/>
       <c r="D625" t="inlineStr">
         <is>
-          <t>[[   0.84521463    0.41323674   -1.15612828    1.59519565   -0.69751873]
- [  11.85192769   18.57233411  -76.76256604   92.90109765  -45.56279341]
- [ -61.50772831  146.04271298 -249.63952752  316.38452301 -150.27998017]]</t>
+          <t>[[   0.84468698    0.41342191   -1.15362199    1.59158294   -0.69606983]
+ [  11.83946945   18.59550661  -76.77434856   92.89491016  -45.55553765]
+ [ -61.50598269  145.98142294 -249.51666719  316.31355374 -150.2723268 ]]</t>
         </is>
       </c>
       <c r="E625" t="inlineStr"/>
@@ -16484,7 +16484,7 @@
       <c r="C626" t="inlineStr"/>
       <c r="D626" t="inlineStr">
         <is>
-          <t>[[  4.20589479 -16.78831007  31.31462981 -25.51336868   7.78115416]
+          <t>[[  4.20273043 -16.7720575   31.28424609 -25.48849783   7.7735788 ]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -16509,7 +16509,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>[0.26685509 1.21826429 2.7264098 ]</t>
+          <t>[0.26685824 1.21832108 2.72677859]</t>
         </is>
       </c>
       <c r="E627" t="inlineStr"/>
@@ -16532,7 +16532,7 @@
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>[0.26360487 1.0237949  2.6636403 ]</t>
+          <t>[0.26360761 1.02383396 2.66402667]</t>
         </is>
       </c>
       <c r="E628" t="inlineStr"/>
@@ -16555,7 +16555,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>[4.73558809 0.         0.        ]</t>
+          <t>[4.73549594 0.         0.        ]</t>
         </is>
       </c>
       <c r="E629" t="inlineStr"/>
@@ -16579,18 +16579,18 @@
       <c r="D630" t="inlineStr">
         <is>
           <t>[[0.        ]
- [0.00578381]
- [0.02182723]
- [0.04720153]
- [0.10466023]
- [0.18801562]
- [0.29234876]
- [0.36830246]
- [0.45667622]
- [0.55465968]
- [0.65351988]
- [0.75878785]
- [0.86781665]]</t>
+ [0.00578128]
+ [0.0218177 ]
+ [0.04718091]
+ [0.10462642]
+ [0.18797721]
+ [0.29231272]
+ [0.36826982]
+ [0.4566475 ]
+ [0.55463521]
+ [0.65349936]
+ [0.7587712 ]
+ [0.86780382]]</t>
         </is>
       </c>
       <c r="E630" t="inlineStr"/>
@@ -16613,7 +16613,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>[0.86781665]</t>
+          <t>[0.86780382]</t>
         </is>
       </c>
       <c r="E631" t="inlineStr"/>
@@ -16636,18 +16636,18 @@
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>[[-17675474.04604535]
- [-15579935.09648651]
- [-13483314.45143045]
- [-11815395.94933672]
- [-10146013.48436328]
- [ -8475390.63871807]
- [ -8086781.11118934]
- [ -7697808.89734239]
- [ -7308495.89839982]
- [ -7002671.90023286]
- [ -6740490.2916013 ]
- [ -6521904.15      ]]</t>
+          <t>[[-17675616.2423275 ]
+ [-15579158.26477832]
+ [-13481618.59173192]
+ [-11814249.85498947]
+ [-10145417.15536732]
+ [ -8475344.07507338]
+ [ -8086752.18721936]
+ [ -7697796.62921059]
+ [ -7308499.32078923]
+ [ -7002673.41537894]
+ [ -6740490.66057829]
+ [ -6521904.14999999]]</t>
         </is>
       </c>
       <c r="E632" t="inlineStr"/>
@@ -16670,18 +16670,18 @@
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>[[2912478.11046093]
- [2913368.97104382]
- [2914180.04028183]
- [2914756.09703146]
- [2916012.11928344]
- [2917031.38834743]
- [2913403.03363594]
- [2913637.90766991]
- [2913820.22876347]
- [2913544.10820134]
- [2913407.77523025]
- [2913212.87537518]]</t>
+          <t>[[2912478.11130552]
+ [2913368.97325693]
+ [2914180.04351811]
+ [2914754.54334205]
+ [2916010.56784803]
+ [2917029.83997802]
+ [2913403.03274234]
+ [2913637.91025541]
+ [2913820.23451225]
+ [2913544.18065396]
+ [2913407.83396474]
+ [2913212.92091163]]</t>
         </is>
       </c>
       <c r="E633" t="inlineStr"/>
@@ -16704,18 +16704,18 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>[[-3354.88807516]
- [-3354.38119436]
- [-3353.78198272]
- [-3353.05800832]
- [-3351.37882345]
- [-3349.43236305]
- [-3353.1192241 ]
- [-3352.24685734]
- [-3351.3156365 ]
- [-3351.23778429]
- [-3350.62488113]
- [-3349.66084702]]</t>
+          <t>[[-3354.88807363]
+ [-3354.38119   ]
+ [-3353.78197533]
+ [-3353.05901088]
+ [-3351.3798183 ]
+ [-3349.43334846]
+ [-3353.11900603]
+ [-3352.2466345 ]
+ [-3351.31541167]
+ [-3351.23746102]
+ [-3350.62462325]
+ [-3349.66065387]]</t>
         </is>
       </c>
       <c r="E634" t="inlineStr"/>
@@ -16738,18 +16738,18 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>[[-222818.48080534]
- [-263177.27897981]
- [-303445.42093956]
- [-360741.47095881]
- [-417696.52490672]
- [-474372.03354204]
- [-508201.33172902]
- [-541699.01683295]
- [-574875.34008509]
- [-605506.65431162]
- [-635614.79310258]
- [-664796.34298229]]</t>
+          <t>[[-222819.02440323]
+ [-263177.88259038]
+ [-303446.13652196]
+ [-360742.35133171]
+ [-417697.43838069]
+ [-474372.83378987]
+ [-508201.9983294 ]
+ [-541699.53980934]
+ [-574875.71153478]
+ [-605506.88701382]
+ [-635614.90256503]
+ [-664796.34297475]]</t>
         </is>
       </c>
       <c r="E635" t="inlineStr"/>
@@ -16772,17 +16772,17 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>[[ 3.91556225e+08]
- [ 3.56121148e+08]
- [ 3.20574315e+08]
- [ 2.69584450e+08]
- [ 2.18382917e+08]
- [ 1.67107693e+08]
- [ 1.36333111e+08]
- [ 1.05488617e+08]
- [ 7.46045244e+07]
- [ 4.57608196e+07]
- [ 1.69025028e+07]
+          <t>[[ 3.91555616e+08]
+ [ 3.56120660e+08]
+ [ 3.20574020e+08]
+ [ 2.69584431e+08]
+ [ 2.18383047e+08]
+ [ 1.67107861e+08]
+ [ 1.36333254e+08]
+ [ 1.05488731e+08]
+ [ 7.46046067e+07]
+ [ 4.57608727e+07]
+ [ 1.69025286e+07]
  [-1.19535912e+07]]</t>
         </is>
       </c>
@@ -16806,18 +16806,18 @@
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>[[6490292.62802801]
- [6490216.61756634]
- [6490140.55618992]
- [6490459.59550754]
- [6490350.16947062]
- [6490240.65108298]
- [6491046.46406648]
- [6490978.98919581]
- [6490911.45234288]
- [6491090.65218141]
- [6491269.68007644]
- [6491533.15181504]]</t>
+          <t>[[6490292.35003889]
+ [6490216.3397639 ]
+ [6490140.2785974 ]
+ [6490459.77987847]
+ [6490350.35334112]
+ [6490240.83442098]
+ [6491046.52567378]
+ [6490979.04713555]
+ [6490911.50685135]
+ [6491090.64352078]
+ [6491269.67314822]
+ [6491533.14849952]]</t>
         </is>
       </c>
       <c r="E637" t="inlineStr"/>
@@ -16842,7 +16842,7 @@
         <is>
           <t>[[ 2.91197623e+06]
  [-3.35507584e+03]
- [-1.97695612e+07]]</t>
+ [-1.97706224e+07]]</t>
         </is>
       </c>
       <c r="E638" t="inlineStr"/>
@@ -16865,8 +16865,8 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>[[-1.82360655e+05]
- [ 4.26821057e+08]
+          <t>[[-1.82361183e+05]
+ [ 4.26820404e+08]
  [ 6.48957511e+06]]</t>
         </is>
       </c>
@@ -16890,7 +16890,7 @@
       </c>
       <c r="D640" t="inlineStr">
         <is>
-          <t>[2313919.88767517]</t>
+          <t>[2314027.97109842]</t>
         </is>
       </c>
       <c r="E640" t="inlineStr"/>
@@ -16913,7 +16913,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>[-2.74163489e+00 -3.53965241e-02  9.91864249e+01]</t>
+          <t>[-2.74150683e+00 -3.53948708e-02  9.91792691e+01]</t>
         </is>
       </c>
       <c r="E641" t="inlineStr"/>
@@ -16936,7 +16936,7 @@
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>[3.14386722e+10 3.12942480e+10 2.85379658e+08 2.02613158e+02
+          <t>[3.14380613e+10 3.12936371e+10 2.85382268e+08 2.02613158e+02
  1.08611945e+07 1.44041114e+05]</t>
         </is>
       </c>
@@ -18445,7 +18445,7 @@
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>[2.65900098]</t>
+          <t>[2.66846269]</t>
         </is>
       </c>
       <c r="E695" t="inlineStr"/>
@@ -19604,8 +19604,8 @@
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>[[0.05045858 0.05942742 0.14509201 0.05637616 0.13109693 0.04393484
-  0.12102924]]</t>
+          <t>[[0.05031772 0.0595708  0.14492055 0.05628306 0.13110318 0.04395645
+  0.12123106]]</t>
         </is>
       </c>
       <c r="E738" t="inlineStr">
@@ -19821,7 +19821,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          9.99992573  6.00000003]</t>
+          <t>[10.         10.         10.         10.          6.00000255]</t>
         </is>
       </c>
       <c r="E746" t="inlineStr">
@@ -19871,7 +19871,7 @@
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>[[0.08000787 0.05507333 0.01943857 0.008654   0.01654327]]</t>
+          <t>[[0.08002922 0.055112   0.01937491 0.00871629 0.01648097]]</t>
         </is>
       </c>
       <c r="E748" t="inlineStr">

</xml_diff>

<commit_message>
added monopile check files.
</commit_message>
<xml_diff>
--- a/examples/for_equinor/for_equinor-monopile/15mw/20m/outputs/monotow_output.xlsx
+++ b/examples/for_equinor/for_equinor-monopile/15mw/20m/outputs/monotow_output.xlsx
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>[2.66846269]</t>
+          <t>[2.66842097]</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -17538,7 +17538,7 @@
       </c>
       <c r="D658" t="inlineStr">
         <is>
-          <t>direct_drive</t>
+          <t>geared</t>
         </is>
       </c>
       <c r="E658" t="inlineStr">
@@ -18445,7 +18445,7 @@
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>[2.66846269]</t>
+          <t>[2.66842097]</t>
         </is>
       </c>
       <c r="E695" t="inlineStr"/>

</xml_diff>